<commit_message>
Acutalizado formato de maestría
</commit_message>
<xml_diff>
--- a/public/formato_mae.xlsx
+++ b/public/formato_mae.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web\uc\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D1970E-BBC4-4679-8C2A-529375085E6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A6886B-3B74-4535-97D7-4A46A0ACAC7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="28">
   <si>
     <t>UNIVERSIDAD CIUDADANA DE NUEVO LEÓN</t>
   </si>
@@ -111,6 +111,15 @@
   </si>
   <si>
     <t>Firma Tutor</t>
+  </si>
+  <si>
+    <t>REGULARIZACIÓN</t>
+  </si>
+  <si>
+    <t>APRECIACIÓN</t>
+  </si>
+  <si>
+    <t>AUTO-EVALUACIÓN</t>
   </si>
 </sst>
 </file>
@@ -238,7 +247,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -597,11 +606,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -777,6 +812,19 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -825,6 +873,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -835,6 +889,16 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -847,10 +911,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -884,7 +944,7 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>48283</xdr:rowOff>
+      <xdr:rowOff>42568</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -956,9 +1016,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>197704</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>193894</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>174171</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1007,14 +1067,14 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>48283</xdr:rowOff>
+      <xdr:rowOff>42568</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="1 Imagen">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25C7C1F0-80B8-40B3-80B2-EA44B4DF298C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDB974F8-5760-4727-A3AE-DFD6A5AC5963}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1037,8 +1097,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="28575" y="40005"/>
-          <a:ext cx="1076325" cy="560728"/>
+          <a:off x="30480" y="40005"/>
+          <a:ext cx="1074420" cy="558823"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1079,7 +1139,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>197704</xdr:colOff>
+      <xdr:colOff>193894</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -1088,7 +1148,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66082015-60EE-4141-9921-52EAE20F2713}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0DA52411-1667-429E-BBA4-63329B2C65A8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1103,8 +1163,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6276975" y="47625"/>
-          <a:ext cx="1550254" cy="504825"/>
+          <a:off x="6286500" y="45720"/>
+          <a:ext cx="1542634" cy="510540"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1380,9 +1440,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J74"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:K74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C5" sqref="C5:G5"/>
     </sheetView>
   </sheetViews>
@@ -1397,144 +1460,154 @@
     <col min="12" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="71" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
-      <c r="J1" s="71"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="73" t="s">
+    <row r="3" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="73"/>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73"/>
-      <c r="J3" s="73"/>
-    </row>
-    <row r="4" spans="1:10" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="82"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="82"/>
+    </row>
+    <row r="4" spans="1:11" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
+      <c r="C5" s="83"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="83"/>
+      <c r="G5" s="83"/>
       <c r="H5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="56" t="s">
+      <c r="I5" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="J5" s="56"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J5" s="60"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="59"/>
+      <c r="G6" s="59"/>
       <c r="H6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="75"/>
-      <c r="J6" s="75"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I6" s="79"/>
+      <c r="J6" s="79"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="55"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="59"/>
       <c r="G7" s="7"/>
       <c r="H7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="56"/>
-      <c r="J7" s="56"/>
-    </row>
-    <row r="8" spans="1:10" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I7" s="60"/>
+      <c r="J7" s="60"/>
+    </row>
+    <row r="8" spans="1:11" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10" s="9" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="57" t="s">
+    <row r="9" spans="1:11" s="9" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="59" t="s">
+      <c r="B9" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="61" t="s">
+      <c r="C9" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="63" t="s">
+      <c r="D9" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="65" t="s">
+      <c r="E9" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="67" t="s">
+      <c r="F9" s="77" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="78"/>
+      <c r="H9" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="67" t="s">
+      <c r="I9" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="69" t="s">
+      <c r="J9" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="I9" s="70"/>
-    </row>
-    <row r="10" spans="1:10" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="58"/>
-      <c r="B10" s="60"/>
-      <c r="C10" s="62"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="66"/>
-      <c r="F10" s="68"/>
-      <c r="G10" s="68"/>
-      <c r="H10" s="10" t="s">
+      <c r="K9" s="76"/>
+    </row>
+    <row r="10" spans="1:11" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="62"/>
+      <c r="B10" s="64"/>
+      <c r="C10" s="66"/>
+      <c r="D10" s="68"/>
+      <c r="E10" s="70"/>
+      <c r="F10" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="72"/>
+      <c r="I10" s="74"/>
+      <c r="J10" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="I10" s="11" t="s">
+      <c r="K10" s="11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>1</v>
       </c>
@@ -1542,14 +1615,16 @@
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
       <c r="E11" s="15"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F11" s="55"/>
+      <c r="G11" s="55"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20">
         <v>2</v>
       </c>
@@ -1557,14 +1632,16 @@
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
       <c r="E12" s="23"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F12" s="55"/>
+      <c r="G12" s="55"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20">
         <v>3</v>
       </c>
@@ -1572,14 +1649,16 @@
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
       <c r="E13" s="23"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F13" s="55"/>
+      <c r="G13" s="55"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20">
         <v>4</v>
       </c>
@@ -1587,14 +1666,16 @@
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
       <c r="E14" s="23"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F14" s="55"/>
+      <c r="G14" s="55"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20">
         <v>5</v>
       </c>
@@ -1602,14 +1683,16 @@
       <c r="C15" s="22"/>
       <c r="D15" s="22"/>
       <c r="E15" s="23"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F15" s="55"/>
+      <c r="G15" s="55"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="20">
         <v>6</v>
       </c>
@@ -1617,14 +1700,16 @@
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
       <c r="E16" s="23"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F16" s="55"/>
+      <c r="G16" s="55"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20">
         <v>7</v>
       </c>
@@ -1632,14 +1717,16 @@
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
       <c r="E17" s="23"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F17" s="55"/>
+      <c r="G17" s="55"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="20">
         <v>8</v>
       </c>
@@ -1647,14 +1734,16 @@
       <c r="C18" s="22"/>
       <c r="D18" s="22"/>
       <c r="E18" s="23"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F18" s="55"/>
+      <c r="G18" s="55"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20">
         <v>9</v>
       </c>
@@ -1662,14 +1751,16 @@
       <c r="C19" s="22"/>
       <c r="D19" s="22"/>
       <c r="E19" s="23"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F19" s="55"/>
+      <c r="G19" s="55"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="20">
         <v>10</v>
       </c>
@@ -1677,14 +1768,16 @@
       <c r="C20" s="22"/>
       <c r="D20" s="22"/>
       <c r="E20" s="23"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F20" s="55"/>
+      <c r="G20" s="55"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20">
         <v>11</v>
       </c>
@@ -1692,14 +1785,16 @@
       <c r="C21" s="22"/>
       <c r="D21" s="22"/>
       <c r="E21" s="23"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F21" s="55"/>
+      <c r="G21" s="55"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="20">
         <v>12</v>
       </c>
@@ -1707,14 +1802,16 @@
       <c r="C22" s="22"/>
       <c r="D22" s="22"/>
       <c r="E22" s="23"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F22" s="55"/>
+      <c r="G22" s="55"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="25"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20">
         <v>13</v>
       </c>
@@ -1722,14 +1819,16 @@
       <c r="C23" s="22"/>
       <c r="D23" s="22"/>
       <c r="E23" s="23"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F23" s="55"/>
+      <c r="G23" s="55"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="25"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="20">
         <v>14</v>
       </c>
@@ -1737,14 +1836,16 @@
       <c r="C24" s="29"/>
       <c r="D24" s="29"/>
       <c r="E24" s="30"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F24" s="55"/>
+      <c r="G24" s="55"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="25"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20">
         <v>15</v>
       </c>
@@ -1752,14 +1853,16 @@
       <c r="C25" s="29"/>
       <c r="D25" s="29"/>
       <c r="E25" s="30"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="32"/>
-      <c r="I25" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F25" s="55"/>
+      <c r="G25" s="55"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="20">
         <v>16</v>
       </c>
@@ -1767,14 +1870,16 @@
       <c r="C26" s="29"/>
       <c r="D26" s="29"/>
       <c r="E26" s="33"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="35"/>
-      <c r="I26" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F26" s="55"/>
+      <c r="G26" s="55"/>
+      <c r="H26" s="34"/>
+      <c r="I26" s="27"/>
+      <c r="J26" s="35"/>
+      <c r="K26" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="20">
         <v>17</v>
       </c>
@@ -1782,14 +1887,16 @@
       <c r="C27" s="29"/>
       <c r="D27" s="29"/>
       <c r="E27" s="30"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="32"/>
-      <c r="I27" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F27" s="55"/>
+      <c r="G27" s="55"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="25"/>
+      <c r="J27" s="32"/>
+      <c r="K27" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="20">
         <v>18</v>
       </c>
@@ -1797,14 +1904,16 @@
       <c r="C28" s="29"/>
       <c r="D28" s="29"/>
       <c r="E28" s="33"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="35"/>
-      <c r="I28" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F28" s="55"/>
+      <c r="G28" s="55"/>
+      <c r="H28" s="34"/>
+      <c r="I28" s="27"/>
+      <c r="J28" s="35"/>
+      <c r="K28" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20">
         <v>19</v>
       </c>
@@ -1812,14 +1921,16 @@
       <c r="C29" s="29"/>
       <c r="D29" s="29"/>
       <c r="E29" s="33"/>
-      <c r="F29" s="34"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="35"/>
-      <c r="I29" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F29" s="55"/>
+      <c r="G29" s="55"/>
+      <c r="H29" s="34"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="35"/>
+      <c r="K29" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="20">
         <v>20</v>
       </c>
@@ -1827,14 +1938,16 @@
       <c r="C30" s="29"/>
       <c r="D30" s="29"/>
       <c r="E30" s="33"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="35"/>
-      <c r="I30" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F30" s="55"/>
+      <c r="G30" s="55"/>
+      <c r="H30" s="34"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="35"/>
+      <c r="K30" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20">
         <v>21</v>
       </c>
@@ -1842,14 +1955,16 @@
       <c r="C31" s="29"/>
       <c r="D31" s="29"/>
       <c r="E31" s="33"/>
-      <c r="F31" s="34"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="35"/>
-      <c r="I31" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F31" s="55"/>
+      <c r="G31" s="55"/>
+      <c r="H31" s="34"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="35"/>
+      <c r="K31" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="20">
         <v>22</v>
       </c>
@@ -1857,14 +1972,16 @@
       <c r="C32" s="29"/>
       <c r="D32" s="29"/>
       <c r="E32" s="30"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="25"/>
-      <c r="H32" s="32"/>
-      <c r="I32" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F32" s="55"/>
+      <c r="G32" s="55"/>
+      <c r="H32" s="31"/>
+      <c r="I32" s="25"/>
+      <c r="J32" s="32"/>
+      <c r="K32" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="20">
         <v>23</v>
       </c>
@@ -1872,14 +1989,16 @@
       <c r="C33" s="29"/>
       <c r="D33" s="29"/>
       <c r="E33" s="30"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="25"/>
-      <c r="H33" s="32"/>
-      <c r="I33" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F33" s="55"/>
+      <c r="G33" s="55"/>
+      <c r="H33" s="31"/>
+      <c r="I33" s="25"/>
+      <c r="J33" s="32"/>
+      <c r="K33" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="20">
         <v>24</v>
       </c>
@@ -1887,14 +2006,16 @@
       <c r="C34" s="29"/>
       <c r="D34" s="29"/>
       <c r="E34" s="33"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="27"/>
-      <c r="H34" s="35"/>
-      <c r="I34" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F34" s="55"/>
+      <c r="G34" s="55"/>
+      <c r="H34" s="34"/>
+      <c r="I34" s="27"/>
+      <c r="J34" s="35"/>
+      <c r="K34" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="20">
         <v>25</v>
       </c>
@@ -1902,14 +2023,16 @@
       <c r="C35" s="29"/>
       <c r="D35" s="29"/>
       <c r="E35" s="30"/>
-      <c r="F35" s="31"/>
-      <c r="G35" s="25"/>
-      <c r="H35" s="32"/>
-      <c r="I35" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F35" s="55"/>
+      <c r="G35" s="55"/>
+      <c r="H35" s="31"/>
+      <c r="I35" s="25"/>
+      <c r="J35" s="32"/>
+      <c r="K35" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="20">
         <v>26</v>
       </c>
@@ -1917,14 +2040,16 @@
       <c r="C36" s="29"/>
       <c r="D36" s="29"/>
       <c r="E36" s="33"/>
-      <c r="F36" s="34"/>
-      <c r="G36" s="27"/>
-      <c r="H36" s="35"/>
-      <c r="I36" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F36" s="55"/>
+      <c r="G36" s="55"/>
+      <c r="H36" s="34"/>
+      <c r="I36" s="27"/>
+      <c r="J36" s="35"/>
+      <c r="K36" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20">
         <v>27</v>
       </c>
@@ -1932,14 +2057,16 @@
       <c r="C37" s="29"/>
       <c r="D37" s="29"/>
       <c r="E37" s="33"/>
-      <c r="F37" s="34"/>
-      <c r="G37" s="27"/>
-      <c r="H37" s="35"/>
-      <c r="I37" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F37" s="55"/>
+      <c r="G37" s="55"/>
+      <c r="H37" s="34"/>
+      <c r="I37" s="27"/>
+      <c r="J37" s="35"/>
+      <c r="K37" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="20">
         <v>28</v>
       </c>
@@ -1947,14 +2074,16 @@
       <c r="C38" s="29"/>
       <c r="D38" s="29"/>
       <c r="E38" s="33"/>
-      <c r="F38" s="34"/>
-      <c r="G38" s="27"/>
-      <c r="H38" s="35"/>
-      <c r="I38" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F38" s="55"/>
+      <c r="G38" s="55"/>
+      <c r="H38" s="34"/>
+      <c r="I38" s="27"/>
+      <c r="J38" s="35"/>
+      <c r="K38" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="20">
         <v>29</v>
       </c>
@@ -1962,14 +2091,16 @@
       <c r="C39" s="29"/>
       <c r="D39" s="29"/>
       <c r="E39" s="30"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="25"/>
-      <c r="H39" s="32"/>
-      <c r="I39" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F39" s="55"/>
+      <c r="G39" s="55"/>
+      <c r="H39" s="31"/>
+      <c r="I39" s="25"/>
+      <c r="J39" s="32"/>
+      <c r="K39" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="20">
         <v>30</v>
       </c>
@@ -1977,14 +2108,16 @@
       <c r="C40" s="29"/>
       <c r="D40" s="29"/>
       <c r="E40" s="30"/>
-      <c r="F40" s="31"/>
-      <c r="G40" s="25"/>
-      <c r="H40" s="32"/>
-      <c r="I40" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F40" s="55"/>
+      <c r="G40" s="55"/>
+      <c r="H40" s="31"/>
+      <c r="I40" s="25"/>
+      <c r="J40" s="32"/>
+      <c r="K40" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="20">
         <v>31</v>
       </c>
@@ -1992,14 +2125,16 @@
       <c r="C41" s="29"/>
       <c r="D41" s="29"/>
       <c r="E41" s="30"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="25"/>
-      <c r="H41" s="32"/>
-      <c r="I41" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F41" s="55"/>
+      <c r="G41" s="55"/>
+      <c r="H41" s="31"/>
+      <c r="I41" s="25"/>
+      <c r="J41" s="32"/>
+      <c r="K41" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="20">
         <v>32</v>
       </c>
@@ -2007,14 +2142,16 @@
       <c r="C42" s="29"/>
       <c r="D42" s="29"/>
       <c r="E42" s="33"/>
-      <c r="F42" s="34"/>
-      <c r="G42" s="27"/>
-      <c r="H42" s="35"/>
-      <c r="I42" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F42" s="55"/>
+      <c r="G42" s="55"/>
+      <c r="H42" s="34"/>
+      <c r="I42" s="27"/>
+      <c r="J42" s="35"/>
+      <c r="K42" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="20">
         <v>33</v>
       </c>
@@ -2022,14 +2159,16 @@
       <c r="C43" s="29"/>
       <c r="D43" s="29"/>
       <c r="E43" s="30"/>
-      <c r="F43" s="31"/>
-      <c r="G43" s="25"/>
-      <c r="H43" s="32"/>
-      <c r="I43" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F43" s="55"/>
+      <c r="G43" s="55"/>
+      <c r="H43" s="31"/>
+      <c r="I43" s="25"/>
+      <c r="J43" s="32"/>
+      <c r="K43" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="20">
         <v>34</v>
       </c>
@@ -2037,14 +2176,16 @@
       <c r="C44" s="29"/>
       <c r="D44" s="29"/>
       <c r="E44" s="33"/>
-      <c r="F44" s="34"/>
-      <c r="G44" s="27"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F44" s="55"/>
+      <c r="G44" s="55"/>
+      <c r="H44" s="34"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="35"/>
+      <c r="K44" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="20">
         <v>35</v>
       </c>
@@ -2052,14 +2193,16 @@
       <c r="C45" s="29"/>
       <c r="D45" s="29"/>
       <c r="E45" s="30"/>
-      <c r="F45" s="31"/>
-      <c r="G45" s="25"/>
-      <c r="H45" s="32"/>
-      <c r="I45" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F45" s="55"/>
+      <c r="G45" s="55"/>
+      <c r="H45" s="31"/>
+      <c r="I45" s="25"/>
+      <c r="J45" s="32"/>
+      <c r="K45" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="20">
         <v>36</v>
       </c>
@@ -2067,14 +2210,16 @@
       <c r="C46" s="29"/>
       <c r="D46" s="29"/>
       <c r="E46" s="33"/>
-      <c r="F46" s="34"/>
-      <c r="G46" s="27"/>
-      <c r="H46" s="35"/>
-      <c r="I46" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F46" s="55"/>
+      <c r="G46" s="55"/>
+      <c r="H46" s="34"/>
+      <c r="I46" s="27"/>
+      <c r="J46" s="35"/>
+      <c r="K46" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="20">
         <v>37</v>
       </c>
@@ -2082,14 +2227,16 @@
       <c r="C47" s="29"/>
       <c r="D47" s="29"/>
       <c r="E47" s="33"/>
-      <c r="F47" s="34"/>
-      <c r="G47" s="27"/>
-      <c r="H47" s="35"/>
-      <c r="I47" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F47" s="55"/>
+      <c r="G47" s="55"/>
+      <c r="H47" s="34"/>
+      <c r="I47" s="27"/>
+      <c r="J47" s="35"/>
+      <c r="K47" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="20">
         <v>38</v>
       </c>
@@ -2097,14 +2244,16 @@
       <c r="C48" s="29"/>
       <c r="D48" s="29"/>
       <c r="E48" s="33"/>
-      <c r="F48" s="34"/>
-      <c r="G48" s="27"/>
-      <c r="H48" s="35"/>
-      <c r="I48" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F48" s="55"/>
+      <c r="G48" s="55"/>
+      <c r="H48" s="34"/>
+      <c r="I48" s="27"/>
+      <c r="J48" s="35"/>
+      <c r="K48" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="20">
         <v>39</v>
       </c>
@@ -2112,14 +2261,16 @@
       <c r="C49" s="29"/>
       <c r="D49" s="29"/>
       <c r="E49" s="33"/>
-      <c r="F49" s="34"/>
-      <c r="G49" s="27"/>
-      <c r="H49" s="35"/>
-      <c r="I49" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F49" s="55"/>
+      <c r="G49" s="55"/>
+      <c r="H49" s="34"/>
+      <c r="I49" s="27"/>
+      <c r="J49" s="35"/>
+      <c r="K49" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="20">
         <f>A49+1</f>
         <v>40</v>
@@ -2128,14 +2279,16 @@
       <c r="C50" s="29"/>
       <c r="D50" s="29"/>
       <c r="E50" s="33"/>
-      <c r="F50" s="34"/>
-      <c r="G50" s="27"/>
-      <c r="H50" s="35"/>
-      <c r="I50" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F50" s="55"/>
+      <c r="G50" s="55"/>
+      <c r="H50" s="34"/>
+      <c r="I50" s="27"/>
+      <c r="J50" s="35"/>
+      <c r="K50" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="20">
         <f t="shared" ref="A51:A59" si="0">A50+1</f>
         <v>41</v>
@@ -2144,14 +2297,16 @@
       <c r="C51" s="29"/>
       <c r="D51" s="29"/>
       <c r="E51" s="33"/>
-      <c r="F51" s="34"/>
-      <c r="G51" s="27"/>
-      <c r="H51" s="35"/>
-      <c r="I51" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F51" s="55"/>
+      <c r="G51" s="55"/>
+      <c r="H51" s="34"/>
+      <c r="I51" s="27"/>
+      <c r="J51" s="35"/>
+      <c r="K51" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="20">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -2160,14 +2315,16 @@
       <c r="C52" s="29"/>
       <c r="D52" s="29"/>
       <c r="E52" s="33"/>
-      <c r="F52" s="34"/>
-      <c r="G52" s="27"/>
-      <c r="H52" s="35"/>
-      <c r="I52" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F52" s="55"/>
+      <c r="G52" s="55"/>
+      <c r="H52" s="34"/>
+      <c r="I52" s="27"/>
+      <c r="J52" s="35"/>
+      <c r="K52" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="20">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -2176,14 +2333,16 @@
       <c r="C53" s="29"/>
       <c r="D53" s="29"/>
       <c r="E53" s="33"/>
-      <c r="F53" s="34"/>
-      <c r="G53" s="27"/>
-      <c r="H53" s="35"/>
-      <c r="I53" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F53" s="55"/>
+      <c r="G53" s="55"/>
+      <c r="H53" s="34"/>
+      <c r="I53" s="27"/>
+      <c r="J53" s="35"/>
+      <c r="K53" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="20">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -2192,14 +2351,16 @@
       <c r="C54" s="29"/>
       <c r="D54" s="29"/>
       <c r="E54" s="33"/>
-      <c r="F54" s="34"/>
-      <c r="G54" s="27"/>
-      <c r="H54" s="35"/>
-      <c r="I54" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F54" s="55"/>
+      <c r="G54" s="55"/>
+      <c r="H54" s="34"/>
+      <c r="I54" s="27"/>
+      <c r="J54" s="35"/>
+      <c r="K54" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="20">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -2208,14 +2369,16 @@
       <c r="C55" s="29"/>
       <c r="D55" s="29"/>
       <c r="E55" s="33"/>
-      <c r="F55" s="34"/>
-      <c r="G55" s="27"/>
-      <c r="H55" s="35"/>
-      <c r="I55" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F55" s="55"/>
+      <c r="G55" s="55"/>
+      <c r="H55" s="34"/>
+      <c r="I55" s="27"/>
+      <c r="J55" s="35"/>
+      <c r="K55" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="20">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -2224,14 +2387,16 @@
       <c r="C56" s="29"/>
       <c r="D56" s="29"/>
       <c r="E56" s="33"/>
-      <c r="F56" s="34"/>
-      <c r="G56" s="27"/>
-      <c r="H56" s="35"/>
-      <c r="I56" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F56" s="55"/>
+      <c r="G56" s="55"/>
+      <c r="H56" s="34"/>
+      <c r="I56" s="27"/>
+      <c r="J56" s="35"/>
+      <c r="K56" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="20">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -2240,14 +2405,16 @@
       <c r="C57" s="29"/>
       <c r="D57" s="29"/>
       <c r="E57" s="33"/>
-      <c r="F57" s="34"/>
-      <c r="G57" s="27"/>
-      <c r="H57" s="35"/>
-      <c r="I57" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F57" s="55"/>
+      <c r="G57" s="55"/>
+      <c r="H57" s="34"/>
+      <c r="I57" s="27"/>
+      <c r="J57" s="35"/>
+      <c r="K57" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="20">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -2256,14 +2423,16 @@
       <c r="C58" s="29"/>
       <c r="D58" s="29"/>
       <c r="E58" s="33"/>
-      <c r="F58" s="34"/>
-      <c r="G58" s="27"/>
-      <c r="H58" s="35"/>
-      <c r="I58" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F58" s="55"/>
+      <c r="G58" s="55"/>
+      <c r="H58" s="34"/>
+      <c r="I58" s="27"/>
+      <c r="J58" s="35"/>
+      <c r="K58" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="20">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -2272,14 +2441,16 @@
       <c r="C59" s="29"/>
       <c r="D59" s="29"/>
       <c r="E59" s="33"/>
-      <c r="F59" s="34"/>
-      <c r="G59" s="27"/>
-      <c r="H59" s="35"/>
-      <c r="I59" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F59" s="55"/>
+      <c r="G59" s="55"/>
+      <c r="H59" s="34"/>
+      <c r="I59" s="27"/>
+      <c r="J59" s="35"/>
+      <c r="K59" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="37">
         <v>50</v>
       </c>
@@ -2287,14 +2458,16 @@
       <c r="C60" s="29"/>
       <c r="D60" s="29"/>
       <c r="E60" s="33"/>
-      <c r="F60" s="34"/>
-      <c r="G60" s="27"/>
-      <c r="H60" s="35"/>
-      <c r="I60" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F60" s="55"/>
+      <c r="G60" s="55"/>
+      <c r="H60" s="34"/>
+      <c r="I60" s="27"/>
+      <c r="J60" s="35"/>
+      <c r="K60" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="37">
         <v>51</v>
       </c>
@@ -2302,14 +2475,16 @@
       <c r="C61" s="29"/>
       <c r="D61" s="29"/>
       <c r="E61" s="33"/>
-      <c r="F61" s="34"/>
-      <c r="G61" s="27"/>
-      <c r="H61" s="35"/>
-      <c r="I61" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F61" s="55"/>
+      <c r="G61" s="55"/>
+      <c r="H61" s="34"/>
+      <c r="I61" s="27"/>
+      <c r="J61" s="35"/>
+      <c r="K61" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="37">
         <v>52</v>
       </c>
@@ -2317,14 +2492,16 @@
       <c r="C62" s="29"/>
       <c r="D62" s="29"/>
       <c r="E62" s="33"/>
-      <c r="F62" s="34"/>
-      <c r="G62" s="27"/>
-      <c r="H62" s="35"/>
-      <c r="I62" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F62" s="55"/>
+      <c r="G62" s="55"/>
+      <c r="H62" s="34"/>
+      <c r="I62" s="27"/>
+      <c r="J62" s="35"/>
+      <c r="K62" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="37">
         <v>53</v>
       </c>
@@ -2332,14 +2509,16 @@
       <c r="C63" s="29"/>
       <c r="D63" s="29"/>
       <c r="E63" s="33"/>
-      <c r="F63" s="34"/>
-      <c r="G63" s="27"/>
-      <c r="H63" s="35"/>
-      <c r="I63" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F63" s="55"/>
+      <c r="G63" s="55"/>
+      <c r="H63" s="34"/>
+      <c r="I63" s="27"/>
+      <c r="J63" s="35"/>
+      <c r="K63" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="37">
         <v>54</v>
       </c>
@@ -2347,14 +2526,16 @@
       <c r="C64" s="29"/>
       <c r="D64" s="29"/>
       <c r="E64" s="33"/>
-      <c r="F64" s="34"/>
-      <c r="G64" s="27"/>
-      <c r="H64" s="35"/>
-      <c r="I64" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F64" s="55"/>
+      <c r="G64" s="55"/>
+      <c r="H64" s="34"/>
+      <c r="I64" s="27"/>
+      <c r="J64" s="35"/>
+      <c r="K64" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="37">
         <v>55</v>
       </c>
@@ -2362,14 +2543,16 @@
       <c r="C65" s="29"/>
       <c r="D65" s="29"/>
       <c r="E65" s="33"/>
-      <c r="F65" s="34"/>
-      <c r="G65" s="27"/>
-      <c r="H65" s="35"/>
-      <c r="I65" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F65" s="55"/>
+      <c r="G65" s="55"/>
+      <c r="H65" s="34"/>
+      <c r="I65" s="27"/>
+      <c r="J65" s="35"/>
+      <c r="K65" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="37">
         <v>56</v>
       </c>
@@ -2377,14 +2560,16 @@
       <c r="C66" s="29"/>
       <c r="D66" s="29"/>
       <c r="E66" s="33"/>
-      <c r="F66" s="34"/>
-      <c r="G66" s="27"/>
-      <c r="H66" s="35"/>
-      <c r="I66" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F66" s="55"/>
+      <c r="G66" s="55"/>
+      <c r="H66" s="34"/>
+      <c r="I66" s="27"/>
+      <c r="J66" s="35"/>
+      <c r="K66" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="37">
         <v>57</v>
       </c>
@@ -2392,14 +2577,16 @@
       <c r="C67" s="29"/>
       <c r="D67" s="29"/>
       <c r="E67" s="33"/>
-      <c r="F67" s="34"/>
-      <c r="G67" s="27"/>
-      <c r="H67" s="35"/>
-      <c r="I67" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F67" s="55"/>
+      <c r="G67" s="55"/>
+      <c r="H67" s="34"/>
+      <c r="I67" s="27"/>
+      <c r="J67" s="35"/>
+      <c r="K67" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="37">
         <v>58</v>
       </c>
@@ -2407,14 +2594,16 @@
       <c r="C68" s="29"/>
       <c r="D68" s="29"/>
       <c r="E68" s="33"/>
-      <c r="F68" s="34"/>
-      <c r="G68" s="27"/>
-      <c r="H68" s="35"/>
-      <c r="I68" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F68" s="55"/>
+      <c r="G68" s="55"/>
+      <c r="H68" s="34"/>
+      <c r="I68" s="27"/>
+      <c r="J68" s="35"/>
+      <c r="K68" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="37">
         <v>59</v>
       </c>
@@ -2422,14 +2611,16 @@
       <c r="C69" s="29"/>
       <c r="D69" s="29"/>
       <c r="E69" s="33"/>
-      <c r="F69" s="34"/>
-      <c r="G69" s="27"/>
-      <c r="H69" s="35"/>
-      <c r="I69" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F69" s="55"/>
+      <c r="G69" s="55"/>
+      <c r="H69" s="34"/>
+      <c r="I69" s="27"/>
+      <c r="J69" s="35"/>
+      <c r="K69" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="38">
         <v>60</v>
       </c>
@@ -2437,19 +2628,21 @@
       <c r="C70" s="40"/>
       <c r="D70" s="41"/>
       <c r="E70" s="42"/>
-      <c r="F70" s="43"/>
-      <c r="G70" s="44"/>
-      <c r="H70" s="45"/>
-      <c r="I70" s="46" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="52" t="s">
+      <c r="F70" s="55"/>
+      <c r="G70" s="55"/>
+      <c r="H70" s="43"/>
+      <c r="I70" s="44"/>
+      <c r="J70" s="45"/>
+      <c r="K70" s="46" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="B71" s="52"/>
-      <c r="C71" s="52"/>
+      <c r="B71" s="56"/>
+      <c r="C71" s="56"/>
       <c r="D71" s="47"/>
       <c r="E71" s="48"/>
       <c r="F71" s="48"/>
@@ -2458,7 +2651,7 @@
       <c r="I71" s="2"/>
       <c r="J71" s="2"/>
     </row>
-    <row r="72" spans="1:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D72" s="49" t="s">
         <v>22</v>
       </c>
@@ -2466,29 +2659,29 @@
       <c r="F72" s="49"/>
       <c r="G72" s="49"/>
     </row>
-    <row r="73" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G73" s="50"/>
       <c r="H73" s="50"/>
       <c r="I73" s="50"/>
       <c r="J73" s="50"/>
     </row>
-    <row r="74" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="C74" s="53"/>
-      <c r="D74" s="53"/>
+      <c r="C74" s="57"/>
+      <c r="D74" s="57"/>
       <c r="E74" s="5"/>
       <c r="F74" s="5"/>
-      <c r="G74" s="54" t="s">
+      <c r="G74" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="H74" s="54"/>
-      <c r="I74" s="54"/>
-      <c r="J74" s="54"/>
+      <c r="H74" s="58"/>
+      <c r="I74" s="58"/>
+      <c r="J74" s="58"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="21">
     <mergeCell ref="C6:G6"/>
     <mergeCell ref="I6:J6"/>
     <mergeCell ref="A1:J1"/>
@@ -2506,21 +2699,26 @@
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="F9:G9"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="70" fitToHeight="0" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28BE6F8C-7B43-43A7-AABF-FBD0520EC578}">
-  <dimension ref="A1:J74"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{630E3F86-C72E-4D02-BF08-6D741E5CD31E}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:K74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:G5"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2534,1049 +2732,1189 @@
     <col min="12" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="71" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
-      <c r="J1" s="71"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="73" t="s">
+    <row r="3" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="73"/>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73"/>
-      <c r="J3" s="73"/>
-    </row>
-    <row r="4" spans="1:10" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J4" s="5"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="82"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="82"/>
+    </row>
+    <row r="4" spans="1:11" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J4" s="52"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
+      <c r="C5" s="83"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="83"/>
+      <c r="G5" s="83"/>
       <c r="H5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="56" t="s">
+      <c r="I5" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="J5" s="56"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J5" s="60"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="59"/>
+      <c r="G6" s="59"/>
       <c r="H6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="75"/>
-      <c r="J6" s="75"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I6" s="79"/>
+      <c r="J6" s="79"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="55"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="59"/>
       <c r="G7" s="7"/>
       <c r="H7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="56"/>
-      <c r="J7" s="56"/>
-    </row>
-    <row r="8" spans="1:10" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J8" s="5"/>
-    </row>
-    <row r="9" spans="1:10" s="9" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="57" t="s">
+      <c r="I7" s="60"/>
+      <c r="J7" s="60"/>
+    </row>
+    <row r="8" spans="1:11" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J8" s="52"/>
+    </row>
+    <row r="9" spans="1:11" s="9" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="59" t="s">
+      <c r="B9" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="61" t="s">
+      <c r="C9" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="63" t="s">
+      <c r="D9" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="65" t="s">
+      <c r="E9" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="67" t="s">
+      <c r="F9" s="77" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="78"/>
+      <c r="H9" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="67" t="s">
+      <c r="I9" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="69" t="s">
+      <c r="J9" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="I9" s="70"/>
-    </row>
-    <row r="10" spans="1:10" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="58"/>
-      <c r="B10" s="60"/>
-      <c r="C10" s="62"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="66"/>
-      <c r="F10" s="68"/>
-      <c r="G10" s="68"/>
-      <c r="H10" s="10" t="s">
+      <c r="K9" s="76"/>
+    </row>
+    <row r="10" spans="1:11" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="62"/>
+      <c r="B10" s="64"/>
+      <c r="C10" s="66"/>
+      <c r="D10" s="68"/>
+      <c r="E10" s="70"/>
+      <c r="F10" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="72"/>
+      <c r="I10" s="74"/>
+      <c r="J10" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="I10" s="11" t="s">
+      <c r="K10" s="11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
-        <v>61</v>
+        <v>1</v>
       </c>
       <c r="B11" s="13"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
       <c r="E11" s="15"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F11" s="55"/>
+      <c r="G11" s="55"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20">
-        <v>62</v>
+        <v>2</v>
       </c>
       <c r="B12" s="21"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
       <c r="E12" s="23"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12">
-        <v>63</v>
+      <c r="F12" s="55"/>
+      <c r="G12" s="55"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="20">
+        <v>3</v>
       </c>
       <c r="B13" s="21"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
       <c r="E13" s="23"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F13" s="55"/>
+      <c r="G13" s="55"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="B14" s="21"/>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
       <c r="E14" s="23"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="12">
-        <v>65</v>
+      <c r="F14" s="55"/>
+      <c r="G14" s="55"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="20">
+        <v>5</v>
       </c>
       <c r="B15" s="21"/>
       <c r="C15" s="22"/>
       <c r="D15" s="22"/>
       <c r="E15" s="23"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F15" s="55"/>
+      <c r="G15" s="55"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="20">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="B16" s="21"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
       <c r="E16" s="23"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="12">
-        <v>67</v>
+      <c r="F16" s="55"/>
+      <c r="G16" s="55"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="20">
+        <v>7</v>
       </c>
       <c r="B17" s="21"/>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
       <c r="E17" s="23"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F17" s="55"/>
+      <c r="G17" s="55"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="20">
-        <v>68</v>
+        <v>8</v>
       </c>
       <c r="B18" s="21"/>
       <c r="C18" s="22"/>
       <c r="D18" s="22"/>
       <c r="E18" s="23"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="12">
-        <v>69</v>
+      <c r="F18" s="55"/>
+      <c r="G18" s="55"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="20">
+        <v>9</v>
       </c>
       <c r="B19" s="21"/>
       <c r="C19" s="22"/>
       <c r="D19" s="22"/>
       <c r="E19" s="23"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F19" s="55"/>
+      <c r="G19" s="55"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="20">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="B20" s="21"/>
       <c r="C20" s="22"/>
       <c r="D20" s="22"/>
       <c r="E20" s="23"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="12">
-        <v>71</v>
+      <c r="F20" s="55"/>
+      <c r="G20" s="55"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="20">
+        <v>11</v>
       </c>
       <c r="B21" s="21"/>
       <c r="C21" s="22"/>
       <c r="D21" s="22"/>
       <c r="E21" s="23"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F21" s="55"/>
+      <c r="G21" s="55"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="20">
-        <v>72</v>
+        <v>12</v>
       </c>
       <c r="B22" s="21"/>
       <c r="C22" s="22"/>
       <c r="D22" s="22"/>
       <c r="E22" s="23"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="12">
-        <v>73</v>
+      <c r="F22" s="55"/>
+      <c r="G22" s="55"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="25"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="20">
+        <v>13</v>
       </c>
       <c r="B23" s="21"/>
       <c r="C23" s="22"/>
       <c r="D23" s="22"/>
       <c r="E23" s="23"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F23" s="55"/>
+      <c r="G23" s="55"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="25"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="20">
-        <v>74</v>
+        <v>14</v>
       </c>
       <c r="B24" s="28"/>
       <c r="C24" s="29"/>
       <c r="D24" s="29"/>
       <c r="E24" s="30"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="12">
-        <v>75</v>
+      <c r="F24" s="55"/>
+      <c r="G24" s="55"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="25"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="20">
+        <v>15</v>
       </c>
       <c r="B25" s="28"/>
       <c r="C25" s="29"/>
       <c r="D25" s="29"/>
       <c r="E25" s="30"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="32"/>
-      <c r="I25" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F25" s="55"/>
+      <c r="G25" s="55"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="20">
-        <v>76</v>
+        <v>16</v>
       </c>
       <c r="B26" s="28"/>
       <c r="C26" s="29"/>
       <c r="D26" s="29"/>
       <c r="E26" s="33"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="35"/>
-      <c r="I26" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="12">
-        <v>77</v>
+      <c r="F26" s="55"/>
+      <c r="G26" s="55"/>
+      <c r="H26" s="34"/>
+      <c r="I26" s="27"/>
+      <c r="J26" s="35"/>
+      <c r="K26" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="20">
+        <v>17</v>
       </c>
       <c r="B27" s="28"/>
       <c r="C27" s="29"/>
       <c r="D27" s="29"/>
       <c r="E27" s="30"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="32"/>
-      <c r="I27" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F27" s="55"/>
+      <c r="G27" s="55"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="25"/>
+      <c r="J27" s="32"/>
+      <c r="K27" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="20">
-        <v>78</v>
+        <v>18</v>
       </c>
       <c r="B28" s="28"/>
       <c r="C28" s="29"/>
       <c r="D28" s="29"/>
       <c r="E28" s="33"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="35"/>
-      <c r="I28" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="12">
-        <v>79</v>
+      <c r="F28" s="55"/>
+      <c r="G28" s="55"/>
+      <c r="H28" s="34"/>
+      <c r="I28" s="27"/>
+      <c r="J28" s="35"/>
+      <c r="K28" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="20">
+        <v>19</v>
       </c>
       <c r="B29" s="28"/>
       <c r="C29" s="29"/>
       <c r="D29" s="29"/>
       <c r="E29" s="33"/>
-      <c r="F29" s="34"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="35"/>
-      <c r="I29" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F29" s="55"/>
+      <c r="G29" s="55"/>
+      <c r="H29" s="34"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="35"/>
+      <c r="K29" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="20">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="B30" s="28"/>
       <c r="C30" s="29"/>
       <c r="D30" s="29"/>
       <c r="E30" s="33"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="35"/>
-      <c r="I30" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="12">
-        <v>81</v>
+      <c r="F30" s="55"/>
+      <c r="G30" s="55"/>
+      <c r="H30" s="34"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="35"/>
+      <c r="K30" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="20">
+        <v>21</v>
       </c>
       <c r="B31" s="28"/>
       <c r="C31" s="29"/>
       <c r="D31" s="29"/>
       <c r="E31" s="33"/>
-      <c r="F31" s="34"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="35"/>
-      <c r="I31" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F31" s="55"/>
+      <c r="G31" s="55"/>
+      <c r="H31" s="34"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="35"/>
+      <c r="K31" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="20">
-        <v>82</v>
+        <v>22</v>
       </c>
       <c r="B32" s="28"/>
       <c r="C32" s="29"/>
       <c r="D32" s="29"/>
       <c r="E32" s="30"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="25"/>
-      <c r="H32" s="32"/>
-      <c r="I32" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="12">
-        <v>83</v>
+      <c r="F32" s="55"/>
+      <c r="G32" s="55"/>
+      <c r="H32" s="31"/>
+      <c r="I32" s="25"/>
+      <c r="J32" s="32"/>
+      <c r="K32" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="20">
+        <v>23</v>
       </c>
       <c r="B33" s="28"/>
       <c r="C33" s="29"/>
       <c r="D33" s="29"/>
       <c r="E33" s="30"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="25"/>
-      <c r="H33" s="32"/>
-      <c r="I33" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F33" s="55"/>
+      <c r="G33" s="55"/>
+      <c r="H33" s="31"/>
+      <c r="I33" s="25"/>
+      <c r="J33" s="32"/>
+      <c r="K33" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="20">
-        <v>84</v>
+        <v>24</v>
       </c>
       <c r="B34" s="28"/>
       <c r="C34" s="29"/>
       <c r="D34" s="29"/>
       <c r="E34" s="33"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="27"/>
-      <c r="H34" s="35"/>
-      <c r="I34" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="12">
-        <v>85</v>
+      <c r="F34" s="55"/>
+      <c r="G34" s="55"/>
+      <c r="H34" s="34"/>
+      <c r="I34" s="27"/>
+      <c r="J34" s="35"/>
+      <c r="K34" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="20">
+        <v>25</v>
       </c>
       <c r="B35" s="28"/>
       <c r="C35" s="29"/>
       <c r="D35" s="29"/>
       <c r="E35" s="30"/>
-      <c r="F35" s="31"/>
-      <c r="G35" s="25"/>
-      <c r="H35" s="32"/>
-      <c r="I35" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F35" s="55"/>
+      <c r="G35" s="55"/>
+      <c r="H35" s="31"/>
+      <c r="I35" s="25"/>
+      <c r="J35" s="32"/>
+      <c r="K35" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="20">
-        <v>86</v>
+        <v>26</v>
       </c>
       <c r="B36" s="28"/>
       <c r="C36" s="29"/>
       <c r="D36" s="29"/>
       <c r="E36" s="33"/>
-      <c r="F36" s="34"/>
-      <c r="G36" s="27"/>
-      <c r="H36" s="35"/>
-      <c r="I36" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="12">
-        <v>87</v>
+      <c r="F36" s="55"/>
+      <c r="G36" s="55"/>
+      <c r="H36" s="34"/>
+      <c r="I36" s="27"/>
+      <c r="J36" s="35"/>
+      <c r="K36" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="20">
+        <v>27</v>
       </c>
       <c r="B37" s="28"/>
       <c r="C37" s="29"/>
       <c r="D37" s="29"/>
       <c r="E37" s="33"/>
-      <c r="F37" s="34"/>
-      <c r="G37" s="27"/>
-      <c r="H37" s="35"/>
-      <c r="I37" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F37" s="55"/>
+      <c r="G37" s="55"/>
+      <c r="H37" s="34"/>
+      <c r="I37" s="27"/>
+      <c r="J37" s="35"/>
+      <c r="K37" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="20">
-        <v>88</v>
+        <v>28</v>
       </c>
       <c r="B38" s="28"/>
       <c r="C38" s="29"/>
       <c r="D38" s="29"/>
       <c r="E38" s="33"/>
-      <c r="F38" s="34"/>
-      <c r="G38" s="27"/>
-      <c r="H38" s="35"/>
-      <c r="I38" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="12">
-        <v>89</v>
+      <c r="F38" s="55"/>
+      <c r="G38" s="55"/>
+      <c r="H38" s="34"/>
+      <c r="I38" s="27"/>
+      <c r="J38" s="35"/>
+      <c r="K38" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="20">
+        <v>29</v>
       </c>
       <c r="B39" s="28"/>
       <c r="C39" s="29"/>
       <c r="D39" s="29"/>
       <c r="E39" s="30"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="25"/>
-      <c r="H39" s="32"/>
-      <c r="I39" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F39" s="55"/>
+      <c r="G39" s="55"/>
+      <c r="H39" s="31"/>
+      <c r="I39" s="25"/>
+      <c r="J39" s="32"/>
+      <c r="K39" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="20">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="B40" s="28"/>
       <c r="C40" s="29"/>
       <c r="D40" s="29"/>
       <c r="E40" s="30"/>
-      <c r="F40" s="31"/>
-      <c r="G40" s="25"/>
-      <c r="H40" s="32"/>
-      <c r="I40" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="12">
-        <v>91</v>
+      <c r="F40" s="55"/>
+      <c r="G40" s="55"/>
+      <c r="H40" s="31"/>
+      <c r="I40" s="25"/>
+      <c r="J40" s="32"/>
+      <c r="K40" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="20">
+        <v>31</v>
       </c>
       <c r="B41" s="28"/>
       <c r="C41" s="29"/>
       <c r="D41" s="29"/>
       <c r="E41" s="30"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="25"/>
-      <c r="H41" s="32"/>
-      <c r="I41" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F41" s="55"/>
+      <c r="G41" s="55"/>
+      <c r="H41" s="31"/>
+      <c r="I41" s="25"/>
+      <c r="J41" s="32"/>
+      <c r="K41" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="20">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="B42" s="28"/>
       <c r="C42" s="29"/>
       <c r="D42" s="29"/>
       <c r="E42" s="33"/>
-      <c r="F42" s="34"/>
-      <c r="G42" s="27"/>
-      <c r="H42" s="35"/>
-      <c r="I42" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="12">
-        <v>93</v>
+      <c r="F42" s="55"/>
+      <c r="G42" s="55"/>
+      <c r="H42" s="34"/>
+      <c r="I42" s="27"/>
+      <c r="J42" s="35"/>
+      <c r="K42" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="20">
+        <v>33</v>
       </c>
       <c r="B43" s="28"/>
       <c r="C43" s="29"/>
       <c r="D43" s="29"/>
       <c r="E43" s="30"/>
-      <c r="F43" s="31"/>
-      <c r="G43" s="25"/>
-      <c r="H43" s="32"/>
-      <c r="I43" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F43" s="55"/>
+      <c r="G43" s="55"/>
+      <c r="H43" s="31"/>
+      <c r="I43" s="25"/>
+      <c r="J43" s="32"/>
+      <c r="K43" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="20">
-        <v>94</v>
+        <v>34</v>
       </c>
       <c r="B44" s="28"/>
       <c r="C44" s="29"/>
       <c r="D44" s="29"/>
       <c r="E44" s="33"/>
-      <c r="F44" s="34"/>
-      <c r="G44" s="27"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="12">
-        <v>95</v>
+      <c r="F44" s="55"/>
+      <c r="G44" s="55"/>
+      <c r="H44" s="34"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="35"/>
+      <c r="K44" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="20">
+        <v>35</v>
       </c>
       <c r="B45" s="28"/>
       <c r="C45" s="29"/>
       <c r="D45" s="29"/>
       <c r="E45" s="30"/>
-      <c r="F45" s="31"/>
-      <c r="G45" s="25"/>
-      <c r="H45" s="32"/>
-      <c r="I45" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F45" s="55"/>
+      <c r="G45" s="55"/>
+      <c r="H45" s="31"/>
+      <c r="I45" s="25"/>
+      <c r="J45" s="32"/>
+      <c r="K45" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="20">
-        <v>96</v>
+        <v>36</v>
       </c>
       <c r="B46" s="36"/>
       <c r="C46" s="29"/>
       <c r="D46" s="29"/>
       <c r="E46" s="33"/>
-      <c r="F46" s="34"/>
-      <c r="G46" s="27"/>
-      <c r="H46" s="35"/>
-      <c r="I46" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="12">
-        <v>97</v>
+      <c r="F46" s="55"/>
+      <c r="G46" s="55"/>
+      <c r="H46" s="34"/>
+      <c r="I46" s="27"/>
+      <c r="J46" s="35"/>
+      <c r="K46" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="20">
+        <v>37</v>
       </c>
       <c r="B47" s="36"/>
       <c r="C47" s="29"/>
       <c r="D47" s="29"/>
       <c r="E47" s="33"/>
-      <c r="F47" s="34"/>
-      <c r="G47" s="27"/>
-      <c r="H47" s="35"/>
-      <c r="I47" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F47" s="55"/>
+      <c r="G47" s="55"/>
+      <c r="H47" s="34"/>
+      <c r="I47" s="27"/>
+      <c r="J47" s="35"/>
+      <c r="K47" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="20">
-        <v>98</v>
+        <v>38</v>
       </c>
       <c r="B48" s="36"/>
       <c r="C48" s="29"/>
       <c r="D48" s="29"/>
       <c r="E48" s="33"/>
-      <c r="F48" s="34"/>
-      <c r="G48" s="27"/>
-      <c r="H48" s="35"/>
-      <c r="I48" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="12">
-        <v>99</v>
+      <c r="F48" s="55"/>
+      <c r="G48" s="55"/>
+      <c r="H48" s="34"/>
+      <c r="I48" s="27"/>
+      <c r="J48" s="35"/>
+      <c r="K48" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="20">
+        <v>39</v>
       </c>
       <c r="B49" s="36"/>
       <c r="C49" s="29"/>
       <c r="D49" s="29"/>
       <c r="E49" s="33"/>
-      <c r="F49" s="34"/>
-      <c r="G49" s="27"/>
-      <c r="H49" s="35"/>
-      <c r="I49" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F49" s="55"/>
+      <c r="G49" s="55"/>
+      <c r="H49" s="34"/>
+      <c r="I49" s="27"/>
+      <c r="J49" s="35"/>
+      <c r="K49" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="20">
-        <v>100</v>
+        <f>A49+1</f>
+        <v>40</v>
       </c>
       <c r="B50" s="36"/>
       <c r="C50" s="29"/>
       <c r="D50" s="29"/>
       <c r="E50" s="33"/>
-      <c r="F50" s="34"/>
-      <c r="G50" s="27"/>
-      <c r="H50" s="35"/>
-      <c r="I50" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="12">
-        <v>101</v>
+      <c r="F50" s="55"/>
+      <c r="G50" s="55"/>
+      <c r="H50" s="34"/>
+      <c r="I50" s="27"/>
+      <c r="J50" s="35"/>
+      <c r="K50" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="20">
+        <f t="shared" ref="A51:A59" si="0">A50+1</f>
+        <v>41</v>
       </c>
       <c r="B51" s="36"/>
       <c r="C51" s="29"/>
       <c r="D51" s="29"/>
       <c r="E51" s="33"/>
-      <c r="F51" s="34"/>
-      <c r="G51" s="27"/>
-      <c r="H51" s="35"/>
-      <c r="I51" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F51" s="55"/>
+      <c r="G51" s="55"/>
+      <c r="H51" s="34"/>
+      <c r="I51" s="27"/>
+      <c r="J51" s="35"/>
+      <c r="K51" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="20">
-        <v>102</v>
+        <f t="shared" si="0"/>
+        <v>42</v>
       </c>
       <c r="B52" s="36"/>
       <c r="C52" s="29"/>
       <c r="D52" s="29"/>
       <c r="E52" s="33"/>
-      <c r="F52" s="34"/>
-      <c r="G52" s="27"/>
-      <c r="H52" s="35"/>
-      <c r="I52" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="12">
-        <v>103</v>
+      <c r="F52" s="55"/>
+      <c r="G52" s="55"/>
+      <c r="H52" s="34"/>
+      <c r="I52" s="27"/>
+      <c r="J52" s="35"/>
+      <c r="K52" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="20">
+        <f t="shared" si="0"/>
+        <v>43</v>
       </c>
       <c r="B53" s="36"/>
       <c r="C53" s="29"/>
       <c r="D53" s="29"/>
       <c r="E53" s="33"/>
-      <c r="F53" s="34"/>
-      <c r="G53" s="27"/>
-      <c r="H53" s="35"/>
-      <c r="I53" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F53" s="55"/>
+      <c r="G53" s="55"/>
+      <c r="H53" s="34"/>
+      <c r="I53" s="27"/>
+      <c r="J53" s="35"/>
+      <c r="K53" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="20">
-        <v>104</v>
+        <f t="shared" si="0"/>
+        <v>44</v>
       </c>
       <c r="B54" s="36"/>
       <c r="C54" s="29"/>
       <c r="D54" s="29"/>
       <c r="E54" s="33"/>
-      <c r="F54" s="34"/>
-      <c r="G54" s="27"/>
-      <c r="H54" s="35"/>
-      <c r="I54" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="12">
-        <v>105</v>
+      <c r="F54" s="55"/>
+      <c r="G54" s="55"/>
+      <c r="H54" s="34"/>
+      <c r="I54" s="27"/>
+      <c r="J54" s="35"/>
+      <c r="K54" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="20">
+        <f t="shared" si="0"/>
+        <v>45</v>
       </c>
       <c r="B55" s="36"/>
       <c r="C55" s="29"/>
       <c r="D55" s="29"/>
       <c r="E55" s="33"/>
-      <c r="F55" s="34"/>
-      <c r="G55" s="27"/>
-      <c r="H55" s="35"/>
-      <c r="I55" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F55" s="55"/>
+      <c r="G55" s="55"/>
+      <c r="H55" s="34"/>
+      <c r="I55" s="27"/>
+      <c r="J55" s="35"/>
+      <c r="K55" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="20">
-        <v>106</v>
+        <f t="shared" si="0"/>
+        <v>46</v>
       </c>
       <c r="B56" s="36"/>
       <c r="C56" s="29"/>
       <c r="D56" s="29"/>
       <c r="E56" s="33"/>
-      <c r="F56" s="34"/>
-      <c r="G56" s="27"/>
-      <c r="H56" s="35"/>
-      <c r="I56" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="12">
-        <v>107</v>
+      <c r="F56" s="55"/>
+      <c r="G56" s="55"/>
+      <c r="H56" s="34"/>
+      <c r="I56" s="27"/>
+      <c r="J56" s="35"/>
+      <c r="K56" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="20">
+        <f t="shared" si="0"/>
+        <v>47</v>
       </c>
       <c r="B57" s="36"/>
       <c r="C57" s="29"/>
       <c r="D57" s="29"/>
       <c r="E57" s="33"/>
-      <c r="F57" s="34"/>
-      <c r="G57" s="27"/>
-      <c r="H57" s="35"/>
-      <c r="I57" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F57" s="55"/>
+      <c r="G57" s="55"/>
+      <c r="H57" s="34"/>
+      <c r="I57" s="27"/>
+      <c r="J57" s="35"/>
+      <c r="K57" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="20">
-        <v>108</v>
+        <f t="shared" si="0"/>
+        <v>48</v>
       </c>
       <c r="B58" s="36"/>
       <c r="C58" s="29"/>
       <c r="D58" s="29"/>
       <c r="E58" s="33"/>
-      <c r="F58" s="34"/>
-      <c r="G58" s="27"/>
-      <c r="H58" s="35"/>
-      <c r="I58" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="12">
-        <v>109</v>
+      <c r="F58" s="55"/>
+      <c r="G58" s="55"/>
+      <c r="H58" s="34"/>
+      <c r="I58" s="27"/>
+      <c r="J58" s="35"/>
+      <c r="K58" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="20">
+        <f t="shared" si="0"/>
+        <v>49</v>
       </c>
       <c r="B59" s="36"/>
       <c r="C59" s="29"/>
       <c r="D59" s="29"/>
       <c r="E59" s="33"/>
-      <c r="F59" s="34"/>
-      <c r="G59" s="27"/>
-      <c r="H59" s="35"/>
-      <c r="I59" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="20">
-        <v>110</v>
+      <c r="F59" s="55"/>
+      <c r="G59" s="55"/>
+      <c r="H59" s="34"/>
+      <c r="I59" s="27"/>
+      <c r="J59" s="35"/>
+      <c r="K59" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="37">
+        <v>50</v>
       </c>
       <c r="B60" s="36"/>
       <c r="C60" s="29"/>
       <c r="D60" s="29"/>
       <c r="E60" s="33"/>
-      <c r="F60" s="34"/>
-      <c r="G60" s="27"/>
-      <c r="H60" s="35"/>
-      <c r="I60" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="12">
-        <v>111</v>
+      <c r="F60" s="55"/>
+      <c r="G60" s="55"/>
+      <c r="H60" s="34"/>
+      <c r="I60" s="27"/>
+      <c r="J60" s="35"/>
+      <c r="K60" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="37">
+        <v>51</v>
       </c>
       <c r="B61" s="36"/>
       <c r="C61" s="29"/>
       <c r="D61" s="29"/>
       <c r="E61" s="33"/>
-      <c r="F61" s="34"/>
-      <c r="G61" s="27"/>
-      <c r="H61" s="35"/>
-      <c r="I61" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="20">
-        <v>112</v>
+      <c r="F61" s="55"/>
+      <c r="G61" s="55"/>
+      <c r="H61" s="34"/>
+      <c r="I61" s="27"/>
+      <c r="J61" s="35"/>
+      <c r="K61" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="37">
+        <v>52</v>
       </c>
       <c r="B62" s="36"/>
       <c r="C62" s="29"/>
       <c r="D62" s="29"/>
       <c r="E62" s="33"/>
-      <c r="F62" s="34"/>
-      <c r="G62" s="27"/>
-      <c r="H62" s="35"/>
-      <c r="I62" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="12">
-        <v>113</v>
+      <c r="F62" s="55"/>
+      <c r="G62" s="55"/>
+      <c r="H62" s="34"/>
+      <c r="I62" s="27"/>
+      <c r="J62" s="35"/>
+      <c r="K62" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="37">
+        <v>53</v>
       </c>
       <c r="B63" s="36"/>
       <c r="C63" s="29"/>
       <c r="D63" s="29"/>
       <c r="E63" s="33"/>
-      <c r="F63" s="34"/>
-      <c r="G63" s="27"/>
-      <c r="H63" s="35"/>
-      <c r="I63" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="20">
-        <v>114</v>
+      <c r="F63" s="55"/>
+      <c r="G63" s="55"/>
+      <c r="H63" s="34"/>
+      <c r="I63" s="27"/>
+      <c r="J63" s="35"/>
+      <c r="K63" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="37">
+        <v>54</v>
       </c>
       <c r="B64" s="36"/>
       <c r="C64" s="29"/>
       <c r="D64" s="29"/>
       <c r="E64" s="33"/>
-      <c r="F64" s="34"/>
-      <c r="G64" s="27"/>
-      <c r="H64" s="35"/>
-      <c r="I64" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="12">
-        <v>115</v>
+      <c r="F64" s="55"/>
+      <c r="G64" s="55"/>
+      <c r="H64" s="34"/>
+      <c r="I64" s="27"/>
+      <c r="J64" s="35"/>
+      <c r="K64" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="37">
+        <v>55</v>
       </c>
       <c r="B65" s="36"/>
       <c r="C65" s="29"/>
       <c r="D65" s="29"/>
       <c r="E65" s="33"/>
-      <c r="F65" s="34"/>
-      <c r="G65" s="27"/>
-      <c r="H65" s="35"/>
-      <c r="I65" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="20">
-        <v>116</v>
+      <c r="F65" s="55"/>
+      <c r="G65" s="55"/>
+      <c r="H65" s="34"/>
+      <c r="I65" s="27"/>
+      <c r="J65" s="35"/>
+      <c r="K65" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="37">
+        <v>56</v>
       </c>
       <c r="B66" s="36"/>
       <c r="C66" s="29"/>
       <c r="D66" s="29"/>
       <c r="E66" s="33"/>
-      <c r="F66" s="34"/>
-      <c r="G66" s="27"/>
-      <c r="H66" s="35"/>
-      <c r="I66" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="12">
-        <v>117</v>
+      <c r="F66" s="55"/>
+      <c r="G66" s="55"/>
+      <c r="H66" s="34"/>
+      <c r="I66" s="27"/>
+      <c r="J66" s="35"/>
+      <c r="K66" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="37">
+        <v>57</v>
       </c>
       <c r="B67" s="36"/>
       <c r="C67" s="29"/>
       <c r="D67" s="29"/>
       <c r="E67" s="33"/>
-      <c r="F67" s="34"/>
-      <c r="G67" s="27"/>
-      <c r="H67" s="35"/>
-      <c r="I67" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="20">
-        <v>118</v>
+      <c r="F67" s="55"/>
+      <c r="G67" s="55"/>
+      <c r="H67" s="34"/>
+      <c r="I67" s="27"/>
+      <c r="J67" s="35"/>
+      <c r="K67" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="37">
+        <v>58</v>
       </c>
       <c r="B68" s="36"/>
       <c r="C68" s="29"/>
       <c r="D68" s="29"/>
       <c r="E68" s="33"/>
-      <c r="F68" s="34"/>
-      <c r="G68" s="27"/>
-      <c r="H68" s="35"/>
-      <c r="I68" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="12">
-        <v>119</v>
+      <c r="F68" s="55"/>
+      <c r="G68" s="55"/>
+      <c r="H68" s="34"/>
+      <c r="I68" s="27"/>
+      <c r="J68" s="35"/>
+      <c r="K68" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="37">
+        <v>59</v>
       </c>
       <c r="B69" s="36"/>
       <c r="C69" s="29"/>
       <c r="D69" s="29"/>
       <c r="E69" s="33"/>
-      <c r="F69" s="34"/>
-      <c r="G69" s="27"/>
-      <c r="H69" s="35"/>
-      <c r="I69" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="20">
-        <v>120</v>
+      <c r="F69" s="55"/>
+      <c r="G69" s="55"/>
+      <c r="H69" s="34"/>
+      <c r="I69" s="27"/>
+      <c r="J69" s="35"/>
+      <c r="K69" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="38">
+        <v>60</v>
       </c>
       <c r="B70" s="39"/>
       <c r="C70" s="40"/>
       <c r="D70" s="41"/>
       <c r="E70" s="42"/>
-      <c r="F70" s="43"/>
-      <c r="G70" s="44"/>
-      <c r="H70" s="45"/>
-      <c r="I70" s="46" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="52" t="s">
+      <c r="F70" s="55"/>
+      <c r="G70" s="55"/>
+      <c r="H70" s="43"/>
+      <c r="I70" s="44"/>
+      <c r="J70" s="45"/>
+      <c r="K70" s="46" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="B71" s="52"/>
-      <c r="C71" s="52"/>
+      <c r="B71" s="56"/>
+      <c r="C71" s="56"/>
       <c r="D71" s="47"/>
       <c r="E71" s="48"/>
       <c r="F71" s="48"/>
@@ -3585,7 +3923,7 @@
       <c r="I71" s="2"/>
       <c r="J71" s="2"/>
     </row>
-    <row r="72" spans="1:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D72" s="49" t="s">
         <v>22</v>
       </c>
@@ -3593,29 +3931,29 @@
       <c r="F72" s="49"/>
       <c r="G72" s="49"/>
     </row>
-    <row r="73" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G73" s="50"/>
       <c r="H73" s="50"/>
       <c r="I73" s="50"/>
       <c r="J73" s="50"/>
     </row>
-    <row r="74" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="C74" s="53"/>
-      <c r="D74" s="53"/>
-      <c r="E74" s="5"/>
-      <c r="F74" s="5"/>
-      <c r="G74" s="54" t="s">
+      <c r="C74" s="57"/>
+      <c r="D74" s="57"/>
+      <c r="E74" s="52"/>
+      <c r="F74" s="52"/>
+      <c r="G74" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="H74" s="54"/>
-      <c r="I74" s="54"/>
-      <c r="J74" s="54"/>
+      <c r="H74" s="58"/>
+      <c r="I74" s="58"/>
+      <c r="J74" s="58"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="21">
     <mergeCell ref="C6:G6"/>
     <mergeCell ref="I6:J6"/>
     <mergeCell ref="A1:J1"/>
@@ -3623,6 +3961,7 @@
     <mergeCell ref="A3:J3"/>
     <mergeCell ref="C5:G5"/>
     <mergeCell ref="I5:J5"/>
+    <mergeCell ref="J9:K9"/>
     <mergeCell ref="A71:C71"/>
     <mergeCell ref="C74:D74"/>
     <mergeCell ref="G74:J74"/>
@@ -3633,11 +3972,12 @@
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="84" fitToHeight="0" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Formato actualizado. Errores capturados.
</commit_message>
<xml_diff>
--- a/public/formato_mae.xlsx
+++ b/public/formato_mae.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web\uc\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\ucnl\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C946F88-F194-420A-8EF6-B05040778850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97785CEF-4DA9-4983-8325-F6C3A5869C3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -756,9 +756,6 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -841,23 +838,41 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -912,22 +927,8 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1525,156 +1526,156 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="57"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="58" t="s">
+      <c r="A2" s="56"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="88" t="s">
+      <c r="D2" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
-      <c r="L2" s="57"/>
-      <c r="M2" s="57"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
     </row>
     <row r="3" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="89" t="s">
+      <c r="A3" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="89"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60"/>
-      <c r="M3" s="59"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
+      <c r="J3" s="66"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="58"/>
     </row>
     <row r="4" spans="1:13" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J4" s="62"/>
+      <c r="J4" s="61"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="90"/>
-      <c r="D5" s="90"/>
-      <c r="E5" s="90"/>
-      <c r="F5" s="90"/>
-      <c r="G5" s="90"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
       <c r="H5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="67" t="s">
+      <c r="I5" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="J5" s="67"/>
+      <c r="J5" s="68"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="66"/>
-      <c r="D6" s="66"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="66"/>
-      <c r="G6" s="66"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="62"/>
       <c r="H6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="86"/>
-      <c r="J6" s="86"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="63"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="66"/>
-      <c r="D7" s="66"/>
-      <c r="E7" s="66"/>
-      <c r="F7" s="66"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
       <c r="G7" s="6"/>
       <c r="H7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="67"/>
-      <c r="J7" s="67"/>
+      <c r="I7" s="68"/>
+      <c r="J7" s="68"/>
     </row>
     <row r="8" spans="1:13" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:13" s="8" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="68" t="s">
+      <c r="A9" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="70" t="s">
+      <c r="B9" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="72" t="s">
+      <c r="C9" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="74" t="s">
+      <c r="D9" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="76" t="s">
+      <c r="E9" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="84" t="s">
+      <c r="F9" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="85"/>
-      <c r="H9" s="78" t="s">
+      <c r="G9" s="89"/>
+      <c r="H9" s="82" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="80" t="s">
+      <c r="I9" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="J9" s="82" t="s">
+      <c r="J9" s="86" t="s">
         <v>17</v>
       </c>
-      <c r="K9" s="83"/>
+      <c r="K9" s="87"/>
     </row>
     <row r="10" spans="1:13" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="69"/>
-      <c r="B10" s="71"/>
-      <c r="C10" s="73"/>
-      <c r="D10" s="75"/>
-      <c r="E10" s="77"/>
-      <c r="F10" s="41" t="s">
+      <c r="A10" s="73"/>
+      <c r="B10" s="75"/>
+      <c r="C10" s="77"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="81"/>
+      <c r="F10" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="G10" s="42" t="s">
+      <c r="G10" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="H10" s="79"/>
-      <c r="I10" s="81"/>
+      <c r="H10" s="83"/>
+      <c r="I10" s="85"/>
       <c r="J10" s="9" t="s">
         <v>18</v>
       </c>
@@ -1690,12 +1691,12 @@
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
       <c r="E11" s="14"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
       <c r="H11" s="15"/>
-      <c r="I11" s="47"/>
+      <c r="I11" s="46"/>
       <c r="J11" s="16"/>
-      <c r="K11" s="48" t="s">
+      <c r="K11" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1707,12 +1708,12 @@
       <c r="C12" s="19"/>
       <c r="D12" s="19"/>
       <c r="E12" s="20"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
       <c r="H12" s="21"/>
-      <c r="I12" s="49"/>
+      <c r="I12" s="48"/>
       <c r="J12" s="22"/>
-      <c r="K12" s="48" t="s">
+      <c r="K12" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1724,12 +1725,12 @@
       <c r="C13" s="19"/>
       <c r="D13" s="19"/>
       <c r="E13" s="20"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
       <c r="H13" s="21"/>
-      <c r="I13" s="49"/>
+      <c r="I13" s="48"/>
       <c r="J13" s="22"/>
-      <c r="K13" s="48" t="s">
+      <c r="K13" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1741,12 +1742,12 @@
       <c r="C14" s="19"/>
       <c r="D14" s="19"/>
       <c r="E14" s="20"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
       <c r="H14" s="21"/>
-      <c r="I14" s="49"/>
+      <c r="I14" s="48"/>
       <c r="J14" s="22"/>
-      <c r="K14" s="48" t="s">
+      <c r="K14" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1758,12 +1759,12 @@
       <c r="C15" s="19"/>
       <c r="D15" s="19"/>
       <c r="E15" s="20"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="43"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="42"/>
       <c r="H15" s="21"/>
-      <c r="I15" s="49"/>
+      <c r="I15" s="48"/>
       <c r="J15" s="22"/>
-      <c r="K15" s="48" t="s">
+      <c r="K15" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1775,12 +1776,12 @@
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
       <c r="E16" s="20"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="43"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
       <c r="H16" s="21"/>
       <c r="I16" s="23"/>
       <c r="J16" s="22"/>
-      <c r="K16" s="48" t="s">
+      <c r="K16" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1792,12 +1793,12 @@
       <c r="C17" s="19"/>
       <c r="D17" s="19"/>
       <c r="E17" s="20"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="43"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
       <c r="H17" s="21"/>
       <c r="I17" s="23"/>
       <c r="J17" s="22"/>
-      <c r="K17" s="48" t="s">
+      <c r="K17" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1809,12 +1810,12 @@
       <c r="C18" s="19"/>
       <c r="D18" s="19"/>
       <c r="E18" s="20"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
       <c r="H18" s="21"/>
-      <c r="I18" s="49"/>
+      <c r="I18" s="48"/>
       <c r="J18" s="22"/>
-      <c r="K18" s="48" t="s">
+      <c r="K18" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1826,12 +1827,12 @@
       <c r="C19" s="19"/>
       <c r="D19" s="19"/>
       <c r="E19" s="20"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="42"/>
       <c r="H19" s="21"/>
-      <c r="I19" s="49"/>
+      <c r="I19" s="48"/>
       <c r="J19" s="22"/>
-      <c r="K19" s="48" t="s">
+      <c r="K19" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1843,12 +1844,12 @@
       <c r="C20" s="19"/>
       <c r="D20" s="19"/>
       <c r="E20" s="20"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="43"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="42"/>
       <c r="H20" s="21"/>
-      <c r="I20" s="49"/>
+      <c r="I20" s="48"/>
       <c r="J20" s="22"/>
-      <c r="K20" s="48" t="s">
+      <c r="K20" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1860,12 +1861,12 @@
       <c r="C21" s="19"/>
       <c r="D21" s="19"/>
       <c r="E21" s="20"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="43"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="42"/>
       <c r="H21" s="21"/>
-      <c r="I21" s="49"/>
+      <c r="I21" s="48"/>
       <c r="J21" s="22"/>
-      <c r="K21" s="48" t="s">
+      <c r="K21" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1877,12 +1878,12 @@
       <c r="C22" s="19"/>
       <c r="D22" s="19"/>
       <c r="E22" s="20"/>
-      <c r="F22" s="43"/>
-      <c r="G22" s="43"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="42"/>
       <c r="H22" s="21"/>
-      <c r="I22" s="49"/>
+      <c r="I22" s="48"/>
       <c r="J22" s="22"/>
-      <c r="K22" s="48" t="s">
+      <c r="K22" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1894,12 +1895,12 @@
       <c r="C23" s="19"/>
       <c r="D23" s="19"/>
       <c r="E23" s="20"/>
-      <c r="F23" s="43"/>
-      <c r="G23" s="43"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="42"/>
       <c r="H23" s="21"/>
-      <c r="I23" s="49"/>
+      <c r="I23" s="48"/>
       <c r="J23" s="22"/>
-      <c r="K23" s="48" t="s">
+      <c r="K23" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1907,16 +1908,16 @@
       <c r="A24" s="17">
         <v>14</v>
       </c>
-      <c r="B24" s="50"/>
-      <c r="C24" s="51"/>
-      <c r="D24" s="51"/>
+      <c r="B24" s="49"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="50"/>
       <c r="E24" s="20"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="43"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="42"/>
       <c r="H24" s="21"/>
-      <c r="I24" s="49"/>
-      <c r="J24" s="52"/>
-      <c r="K24" s="48" t="s">
+      <c r="I24" s="48"/>
+      <c r="J24" s="51"/>
+      <c r="K24" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1924,16 +1925,16 @@
       <c r="A25" s="17">
         <v>15</v>
       </c>
-      <c r="B25" s="50"/>
-      <c r="C25" s="51"/>
-      <c r="D25" s="51"/>
+      <c r="B25" s="49"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="50"/>
       <c r="E25" s="20"/>
-      <c r="F25" s="43"/>
-      <c r="G25" s="43"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="42"/>
       <c r="H25" s="21"/>
-      <c r="I25" s="49"/>
-      <c r="J25" s="52"/>
-      <c r="K25" s="48" t="s">
+      <c r="I25" s="48"/>
+      <c r="J25" s="51"/>
+      <c r="K25" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1941,16 +1942,16 @@
       <c r="A26" s="17">
         <v>16</v>
       </c>
-      <c r="B26" s="50"/>
-      <c r="C26" s="51"/>
-      <c r="D26" s="51"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="50"/>
       <c r="E26" s="24"/>
-      <c r="F26" s="43"/>
-      <c r="G26" s="43"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="42"/>
       <c r="H26" s="25"/>
       <c r="I26" s="23"/>
       <c r="J26" s="26"/>
-      <c r="K26" s="48" t="s">
+      <c r="K26" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1958,16 +1959,16 @@
       <c r="A27" s="17">
         <v>17</v>
       </c>
-      <c r="B27" s="50"/>
-      <c r="C27" s="51"/>
-      <c r="D27" s="51"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="50"/>
+      <c r="D27" s="50"/>
       <c r="E27" s="20"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="43"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
       <c r="H27" s="21"/>
-      <c r="I27" s="49"/>
-      <c r="J27" s="52"/>
-      <c r="K27" s="48" t="s">
+      <c r="I27" s="48"/>
+      <c r="J27" s="51"/>
+      <c r="K27" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1975,16 +1976,16 @@
       <c r="A28" s="17">
         <v>18</v>
       </c>
-      <c r="B28" s="50"/>
-      <c r="C28" s="51"/>
-      <c r="D28" s="51"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="50"/>
       <c r="E28" s="24"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
+      <c r="F28" s="42"/>
+      <c r="G28" s="42"/>
       <c r="H28" s="25"/>
       <c r="I28" s="23"/>
       <c r="J28" s="26"/>
-      <c r="K28" s="48" t="s">
+      <c r="K28" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1992,16 +1993,16 @@
       <c r="A29" s="17">
         <v>19</v>
       </c>
-      <c r="B29" s="50"/>
-      <c r="C29" s="51"/>
-      <c r="D29" s="51"/>
+      <c r="B29" s="49"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="50"/>
       <c r="E29" s="24"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="43"/>
+      <c r="F29" s="42"/>
+      <c r="G29" s="42"/>
       <c r="H29" s="25"/>
       <c r="I29" s="23"/>
       <c r="J29" s="26"/>
-      <c r="K29" s="48" t="s">
+      <c r="K29" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2009,16 +2010,16 @@
       <c r="A30" s="17">
         <v>20</v>
       </c>
-      <c r="B30" s="50"/>
-      <c r="C30" s="51"/>
-      <c r="D30" s="51"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="50"/>
+      <c r="D30" s="50"/>
       <c r="E30" s="24"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="43"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="42"/>
       <c r="H30" s="25"/>
       <c r="I30" s="23"/>
       <c r="J30" s="26"/>
-      <c r="K30" s="48" t="s">
+      <c r="K30" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2026,16 +2027,16 @@
       <c r="A31" s="17">
         <v>21</v>
       </c>
-      <c r="B31" s="50"/>
-      <c r="C31" s="51"/>
-      <c r="D31" s="51"/>
+      <c r="B31" s="49"/>
+      <c r="C31" s="50"/>
+      <c r="D31" s="50"/>
       <c r="E31" s="24"/>
-      <c r="F31" s="43"/>
-      <c r="G31" s="43"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="42"/>
       <c r="H31" s="25"/>
       <c r="I31" s="23"/>
       <c r="J31" s="26"/>
-      <c r="K31" s="48" t="s">
+      <c r="K31" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2043,16 +2044,16 @@
       <c r="A32" s="17">
         <v>22</v>
       </c>
-      <c r="B32" s="50"/>
-      <c r="C32" s="51"/>
-      <c r="D32" s="51"/>
+      <c r="B32" s="49"/>
+      <c r="C32" s="50"/>
+      <c r="D32" s="50"/>
       <c r="E32" s="20"/>
-      <c r="F32" s="43"/>
-      <c r="G32" s="43"/>
+      <c r="F32" s="42"/>
+      <c r="G32" s="42"/>
       <c r="H32" s="21"/>
-      <c r="I32" s="49"/>
-      <c r="J32" s="52"/>
-      <c r="K32" s="48" t="s">
+      <c r="I32" s="48"/>
+      <c r="J32" s="51"/>
+      <c r="K32" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2060,16 +2061,16 @@
       <c r="A33" s="17">
         <v>23</v>
       </c>
-      <c r="B33" s="50"/>
-      <c r="C33" s="51"/>
-      <c r="D33" s="51"/>
+      <c r="B33" s="49"/>
+      <c r="C33" s="50"/>
+      <c r="D33" s="50"/>
       <c r="E33" s="20"/>
-      <c r="F33" s="43"/>
-      <c r="G33" s="43"/>
+      <c r="F33" s="42"/>
+      <c r="G33" s="42"/>
       <c r="H33" s="21"/>
-      <c r="I33" s="49"/>
-      <c r="J33" s="52"/>
-      <c r="K33" s="48" t="s">
+      <c r="I33" s="48"/>
+      <c r="J33" s="51"/>
+      <c r="K33" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2077,16 +2078,16 @@
       <c r="A34" s="17">
         <v>24</v>
       </c>
-      <c r="B34" s="50"/>
-      <c r="C34" s="51"/>
-      <c r="D34" s="51"/>
+      <c r="B34" s="49"/>
+      <c r="C34" s="50"/>
+      <c r="D34" s="50"/>
       <c r="E34" s="24"/>
-      <c r="F34" s="43"/>
-      <c r="G34" s="43"/>
+      <c r="F34" s="42"/>
+      <c r="G34" s="42"/>
       <c r="H34" s="25"/>
       <c r="I34" s="23"/>
       <c r="J34" s="26"/>
-      <c r="K34" s="48" t="s">
+      <c r="K34" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2094,16 +2095,16 @@
       <c r="A35" s="17">
         <v>25</v>
       </c>
-      <c r="B35" s="50"/>
-      <c r="C35" s="51"/>
-      <c r="D35" s="51"/>
+      <c r="B35" s="49"/>
+      <c r="C35" s="50"/>
+      <c r="D35" s="50"/>
       <c r="E35" s="20"/>
-      <c r="F35" s="43"/>
-      <c r="G35" s="43"/>
+      <c r="F35" s="42"/>
+      <c r="G35" s="42"/>
       <c r="H35" s="21"/>
-      <c r="I35" s="49"/>
-      <c r="J35" s="52"/>
-      <c r="K35" s="48" t="s">
+      <c r="I35" s="48"/>
+      <c r="J35" s="51"/>
+      <c r="K35" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2111,16 +2112,16 @@
       <c r="A36" s="17">
         <v>26</v>
       </c>
-      <c r="B36" s="50"/>
-      <c r="C36" s="51"/>
-      <c r="D36" s="51"/>
+      <c r="B36" s="49"/>
+      <c r="C36" s="50"/>
+      <c r="D36" s="50"/>
       <c r="E36" s="24"/>
-      <c r="F36" s="43"/>
-      <c r="G36" s="43"/>
+      <c r="F36" s="42"/>
+      <c r="G36" s="42"/>
       <c r="H36" s="25"/>
       <c r="I36" s="23"/>
       <c r="J36" s="26"/>
-      <c r="K36" s="48" t="s">
+      <c r="K36" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2128,16 +2129,16 @@
       <c r="A37" s="17">
         <v>27</v>
       </c>
-      <c r="B37" s="50"/>
-      <c r="C37" s="51"/>
-      <c r="D37" s="51"/>
+      <c r="B37" s="49"/>
+      <c r="C37" s="50"/>
+      <c r="D37" s="50"/>
       <c r="E37" s="24"/>
-      <c r="F37" s="43"/>
-      <c r="G37" s="43"/>
+      <c r="F37" s="42"/>
+      <c r="G37" s="42"/>
       <c r="H37" s="25"/>
       <c r="I37" s="23"/>
       <c r="J37" s="26"/>
-      <c r="K37" s="48" t="s">
+      <c r="K37" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2145,16 +2146,16 @@
       <c r="A38" s="17">
         <v>28</v>
       </c>
-      <c r="B38" s="50"/>
-      <c r="C38" s="51"/>
-      <c r="D38" s="51"/>
+      <c r="B38" s="49"/>
+      <c r="C38" s="50"/>
+      <c r="D38" s="50"/>
       <c r="E38" s="24"/>
-      <c r="F38" s="43"/>
-      <c r="G38" s="43"/>
+      <c r="F38" s="42"/>
+      <c r="G38" s="42"/>
       <c r="H38" s="25"/>
       <c r="I38" s="23"/>
       <c r="J38" s="26"/>
-      <c r="K38" s="48" t="s">
+      <c r="K38" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2162,16 +2163,16 @@
       <c r="A39" s="17">
         <v>29</v>
       </c>
-      <c r="B39" s="50"/>
-      <c r="C39" s="51"/>
-      <c r="D39" s="51"/>
+      <c r="B39" s="49"/>
+      <c r="C39" s="50"/>
+      <c r="D39" s="50"/>
       <c r="E39" s="20"/>
-      <c r="F39" s="43"/>
-      <c r="G39" s="43"/>
+      <c r="F39" s="42"/>
+      <c r="G39" s="42"/>
       <c r="H39" s="21"/>
-      <c r="I39" s="49"/>
-      <c r="J39" s="52"/>
-      <c r="K39" s="48" t="s">
+      <c r="I39" s="48"/>
+      <c r="J39" s="51"/>
+      <c r="K39" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2179,16 +2180,16 @@
       <c r="A40" s="17">
         <v>30</v>
       </c>
-      <c r="B40" s="50"/>
-      <c r="C40" s="51"/>
-      <c r="D40" s="51"/>
+      <c r="B40" s="49"/>
+      <c r="C40" s="50"/>
+      <c r="D40" s="50"/>
       <c r="E40" s="20"/>
-      <c r="F40" s="43"/>
-      <c r="G40" s="43"/>
+      <c r="F40" s="42"/>
+      <c r="G40" s="42"/>
       <c r="H40" s="21"/>
-      <c r="I40" s="49"/>
-      <c r="J40" s="52"/>
-      <c r="K40" s="48" t="s">
+      <c r="I40" s="48"/>
+      <c r="J40" s="51"/>
+      <c r="K40" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2196,16 +2197,16 @@
       <c r="A41" s="17">
         <v>31</v>
       </c>
-      <c r="B41" s="50"/>
-      <c r="C41" s="51"/>
-      <c r="D41" s="51"/>
+      <c r="B41" s="49"/>
+      <c r="C41" s="50"/>
+      <c r="D41" s="50"/>
       <c r="E41" s="20"/>
-      <c r="F41" s="43"/>
-      <c r="G41" s="43"/>
+      <c r="F41" s="42"/>
+      <c r="G41" s="42"/>
       <c r="H41" s="21"/>
-      <c r="I41" s="49"/>
-      <c r="J41" s="52"/>
-      <c r="K41" s="48" t="s">
+      <c r="I41" s="48"/>
+      <c r="J41" s="51"/>
+      <c r="K41" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2213,16 +2214,16 @@
       <c r="A42" s="17">
         <v>32</v>
       </c>
-      <c r="B42" s="50"/>
-      <c r="C42" s="51"/>
-      <c r="D42" s="51"/>
+      <c r="B42" s="49"/>
+      <c r="C42" s="50"/>
+      <c r="D42" s="50"/>
       <c r="E42" s="24"/>
-      <c r="F42" s="43"/>
-      <c r="G42" s="43"/>
+      <c r="F42" s="42"/>
+      <c r="G42" s="42"/>
       <c r="H42" s="25"/>
       <c r="I42" s="23"/>
       <c r="J42" s="26"/>
-      <c r="K42" s="48" t="s">
+      <c r="K42" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2230,16 +2231,16 @@
       <c r="A43" s="17">
         <v>33</v>
       </c>
-      <c r="B43" s="50"/>
-      <c r="C43" s="51"/>
-      <c r="D43" s="51"/>
+      <c r="B43" s="49"/>
+      <c r="C43" s="50"/>
+      <c r="D43" s="50"/>
       <c r="E43" s="20"/>
-      <c r="F43" s="43"/>
-      <c r="G43" s="43"/>
+      <c r="F43" s="42"/>
+      <c r="G43" s="42"/>
       <c r="H43" s="21"/>
-      <c r="I43" s="49"/>
-      <c r="J43" s="52"/>
-      <c r="K43" s="48" t="s">
+      <c r="I43" s="48"/>
+      <c r="J43" s="51"/>
+      <c r="K43" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2247,16 +2248,16 @@
       <c r="A44" s="17">
         <v>34</v>
       </c>
-      <c r="B44" s="50"/>
-      <c r="C44" s="51"/>
-      <c r="D44" s="51"/>
+      <c r="B44" s="49"/>
+      <c r="C44" s="50"/>
+      <c r="D44" s="50"/>
       <c r="E44" s="24"/>
-      <c r="F44" s="43"/>
-      <c r="G44" s="43"/>
+      <c r="F44" s="42"/>
+      <c r="G44" s="42"/>
       <c r="H44" s="25"/>
       <c r="I44" s="23"/>
       <c r="J44" s="26"/>
-      <c r="K44" s="48" t="s">
+      <c r="K44" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2264,16 +2265,16 @@
       <c r="A45" s="17">
         <v>35</v>
       </c>
-      <c r="B45" s="50"/>
-      <c r="C45" s="51"/>
-      <c r="D45" s="51"/>
+      <c r="B45" s="49"/>
+      <c r="C45" s="50"/>
+      <c r="D45" s="50"/>
       <c r="E45" s="20"/>
-      <c r="F45" s="43"/>
-      <c r="G45" s="43"/>
+      <c r="F45" s="42"/>
+      <c r="G45" s="42"/>
       <c r="H45" s="21"/>
-      <c r="I45" s="49"/>
-      <c r="J45" s="52"/>
-      <c r="K45" s="48" t="s">
+      <c r="I45" s="48"/>
+      <c r="J45" s="51"/>
+      <c r="K45" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2282,15 +2283,15 @@
         <v>36</v>
       </c>
       <c r="B46" s="27"/>
-      <c r="C46" s="51"/>
-      <c r="D46" s="51"/>
+      <c r="C46" s="50"/>
+      <c r="D46" s="50"/>
       <c r="E46" s="24"/>
-      <c r="F46" s="43"/>
-      <c r="G46" s="43"/>
+      <c r="F46" s="42"/>
+      <c r="G46" s="42"/>
       <c r="H46" s="25"/>
       <c r="I46" s="23"/>
       <c r="J46" s="26"/>
-      <c r="K46" s="48" t="s">
+      <c r="K46" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2299,15 +2300,15 @@
         <v>37</v>
       </c>
       <c r="B47" s="27"/>
-      <c r="C47" s="51"/>
-      <c r="D47" s="51"/>
+      <c r="C47" s="50"/>
+      <c r="D47" s="50"/>
       <c r="E47" s="24"/>
-      <c r="F47" s="43"/>
-      <c r="G47" s="43"/>
+      <c r="F47" s="42"/>
+      <c r="G47" s="42"/>
       <c r="H47" s="25"/>
       <c r="I47" s="23"/>
       <c r="J47" s="26"/>
-      <c r="K47" s="48" t="s">
+      <c r="K47" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2316,15 +2317,15 @@
         <v>38</v>
       </c>
       <c r="B48" s="27"/>
-      <c r="C48" s="51"/>
-      <c r="D48" s="51"/>
+      <c r="C48" s="50"/>
+      <c r="D48" s="50"/>
       <c r="E48" s="24"/>
-      <c r="F48" s="43"/>
-      <c r="G48" s="43"/>
+      <c r="F48" s="42"/>
+      <c r="G48" s="42"/>
       <c r="H48" s="25"/>
       <c r="I48" s="23"/>
       <c r="J48" s="26"/>
-      <c r="K48" s="48" t="s">
+      <c r="K48" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2333,15 +2334,15 @@
         <v>39</v>
       </c>
       <c r="B49" s="27"/>
-      <c r="C49" s="51"/>
-      <c r="D49" s="51"/>
+      <c r="C49" s="50"/>
+      <c r="D49" s="50"/>
       <c r="E49" s="24"/>
-      <c r="F49" s="43"/>
-      <c r="G49" s="43"/>
+      <c r="F49" s="42"/>
+      <c r="G49" s="42"/>
       <c r="H49" s="25"/>
       <c r="I49" s="23"/>
       <c r="J49" s="26"/>
-      <c r="K49" s="48" t="s">
+      <c r="K49" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2351,15 +2352,15 @@
         <v>40</v>
       </c>
       <c r="B50" s="27"/>
-      <c r="C50" s="51"/>
-      <c r="D50" s="51"/>
+      <c r="C50" s="50"/>
+      <c r="D50" s="50"/>
       <c r="E50" s="24"/>
-      <c r="F50" s="43"/>
-      <c r="G50" s="43"/>
+      <c r="F50" s="42"/>
+      <c r="G50" s="42"/>
       <c r="H50" s="25"/>
       <c r="I50" s="23"/>
       <c r="J50" s="26"/>
-      <c r="K50" s="48" t="s">
+      <c r="K50" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2369,15 +2370,15 @@
         <v>41</v>
       </c>
       <c r="B51" s="27"/>
-      <c r="C51" s="51"/>
-      <c r="D51" s="51"/>
+      <c r="C51" s="50"/>
+      <c r="D51" s="50"/>
       <c r="E51" s="24"/>
-      <c r="F51" s="43"/>
-      <c r="G51" s="43"/>
+      <c r="F51" s="42"/>
+      <c r="G51" s="42"/>
       <c r="H51" s="25"/>
       <c r="I51" s="23"/>
       <c r="J51" s="26"/>
-      <c r="K51" s="48" t="s">
+      <c r="K51" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2387,15 +2388,15 @@
         <v>42</v>
       </c>
       <c r="B52" s="27"/>
-      <c r="C52" s="51"/>
-      <c r="D52" s="51"/>
+      <c r="C52" s="50"/>
+      <c r="D52" s="50"/>
       <c r="E52" s="24"/>
-      <c r="F52" s="43"/>
-      <c r="G52" s="43"/>
+      <c r="F52" s="42"/>
+      <c r="G52" s="42"/>
       <c r="H52" s="25"/>
       <c r="I52" s="23"/>
       <c r="J52" s="26"/>
-      <c r="K52" s="48" t="s">
+      <c r="K52" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2405,15 +2406,15 @@
         <v>43</v>
       </c>
       <c r="B53" s="27"/>
-      <c r="C53" s="51"/>
-      <c r="D53" s="51"/>
+      <c r="C53" s="50"/>
+      <c r="D53" s="50"/>
       <c r="E53" s="24"/>
-      <c r="F53" s="43"/>
-      <c r="G53" s="43"/>
+      <c r="F53" s="42"/>
+      <c r="G53" s="42"/>
       <c r="H53" s="25"/>
       <c r="I53" s="23"/>
       <c r="J53" s="26"/>
-      <c r="K53" s="48" t="s">
+      <c r="K53" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2423,15 +2424,15 @@
         <v>44</v>
       </c>
       <c r="B54" s="27"/>
-      <c r="C54" s="51"/>
-      <c r="D54" s="51"/>
+      <c r="C54" s="50"/>
+      <c r="D54" s="50"/>
       <c r="E54" s="24"/>
-      <c r="F54" s="43"/>
-      <c r="G54" s="43"/>
+      <c r="F54" s="42"/>
+      <c r="G54" s="42"/>
       <c r="H54" s="25"/>
       <c r="I54" s="23"/>
       <c r="J54" s="26"/>
-      <c r="K54" s="48" t="s">
+      <c r="K54" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2441,15 +2442,15 @@
         <v>45</v>
       </c>
       <c r="B55" s="27"/>
-      <c r="C55" s="51"/>
-      <c r="D55" s="51"/>
+      <c r="C55" s="50"/>
+      <c r="D55" s="50"/>
       <c r="E55" s="24"/>
-      <c r="F55" s="43"/>
-      <c r="G55" s="43"/>
+      <c r="F55" s="42"/>
+      <c r="G55" s="42"/>
       <c r="H55" s="25"/>
       <c r="I55" s="23"/>
       <c r="J55" s="26"/>
-      <c r="K55" s="48" t="s">
+      <c r="K55" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2459,15 +2460,15 @@
         <v>46</v>
       </c>
       <c r="B56" s="27"/>
-      <c r="C56" s="51"/>
-      <c r="D56" s="51"/>
+      <c r="C56" s="50"/>
+      <c r="D56" s="50"/>
       <c r="E56" s="24"/>
-      <c r="F56" s="43"/>
-      <c r="G56" s="43"/>
+      <c r="F56" s="42"/>
+      <c r="G56" s="42"/>
       <c r="H56" s="25"/>
       <c r="I56" s="23"/>
       <c r="J56" s="26"/>
-      <c r="K56" s="48" t="s">
+      <c r="K56" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2477,15 +2478,15 @@
         <v>47</v>
       </c>
       <c r="B57" s="27"/>
-      <c r="C57" s="51"/>
-      <c r="D57" s="51"/>
+      <c r="C57" s="50"/>
+      <c r="D57" s="50"/>
       <c r="E57" s="24"/>
-      <c r="F57" s="43"/>
-      <c r="G57" s="43"/>
+      <c r="F57" s="42"/>
+      <c r="G57" s="42"/>
       <c r="H57" s="25"/>
       <c r="I57" s="23"/>
       <c r="J57" s="26"/>
-      <c r="K57" s="48" t="s">
+      <c r="K57" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2495,15 +2496,15 @@
         <v>48</v>
       </c>
       <c r="B58" s="27"/>
-      <c r="C58" s="51"/>
-      <c r="D58" s="51"/>
+      <c r="C58" s="50"/>
+      <c r="D58" s="50"/>
       <c r="E58" s="24"/>
-      <c r="F58" s="43"/>
-      <c r="G58" s="43"/>
+      <c r="F58" s="42"/>
+      <c r="G58" s="42"/>
       <c r="H58" s="25"/>
       <c r="I58" s="23"/>
       <c r="J58" s="26"/>
-      <c r="K58" s="48" t="s">
+      <c r="K58" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2513,15 +2514,15 @@
         <v>49</v>
       </c>
       <c r="B59" s="27"/>
-      <c r="C59" s="51"/>
-      <c r="D59" s="51"/>
+      <c r="C59" s="50"/>
+      <c r="D59" s="50"/>
       <c r="E59" s="24"/>
-      <c r="F59" s="43"/>
-      <c r="G59" s="43"/>
+      <c r="F59" s="42"/>
+      <c r="G59" s="42"/>
       <c r="H59" s="25"/>
       <c r="I59" s="23"/>
       <c r="J59" s="26"/>
-      <c r="K59" s="48" t="s">
+      <c r="K59" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2530,15 +2531,15 @@
         <v>50</v>
       </c>
       <c r="B60" s="27"/>
-      <c r="C60" s="51"/>
-      <c r="D60" s="51"/>
+      <c r="C60" s="50"/>
+      <c r="D60" s="50"/>
       <c r="E60" s="24"/>
-      <c r="F60" s="43"/>
-      <c r="G60" s="43"/>
+      <c r="F60" s="42"/>
+      <c r="G60" s="42"/>
       <c r="H60" s="25"/>
       <c r="I60" s="23"/>
       <c r="J60" s="26"/>
-      <c r="K60" s="48" t="s">
+      <c r="K60" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2547,15 +2548,15 @@
         <v>51</v>
       </c>
       <c r="B61" s="27"/>
-      <c r="C61" s="51"/>
-      <c r="D61" s="51"/>
+      <c r="C61" s="50"/>
+      <c r="D61" s="50"/>
       <c r="E61" s="24"/>
-      <c r="F61" s="43"/>
-      <c r="G61" s="43"/>
+      <c r="F61" s="42"/>
+      <c r="G61" s="42"/>
       <c r="H61" s="25"/>
       <c r="I61" s="23"/>
       <c r="J61" s="26"/>
-      <c r="K61" s="48" t="s">
+      <c r="K61" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2564,15 +2565,15 @@
         <v>52</v>
       </c>
       <c r="B62" s="27"/>
-      <c r="C62" s="51"/>
-      <c r="D62" s="51"/>
+      <c r="C62" s="50"/>
+      <c r="D62" s="50"/>
       <c r="E62" s="24"/>
-      <c r="F62" s="43"/>
-      <c r="G62" s="43"/>
+      <c r="F62" s="42"/>
+      <c r="G62" s="42"/>
       <c r="H62" s="25"/>
       <c r="I62" s="23"/>
       <c r="J62" s="26"/>
-      <c r="K62" s="48" t="s">
+      <c r="K62" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2581,15 +2582,15 @@
         <v>53</v>
       </c>
       <c r="B63" s="27"/>
-      <c r="C63" s="51"/>
-      <c r="D63" s="51"/>
+      <c r="C63" s="50"/>
+      <c r="D63" s="50"/>
       <c r="E63" s="24"/>
-      <c r="F63" s="43"/>
-      <c r="G63" s="43"/>
+      <c r="F63" s="42"/>
+      <c r="G63" s="42"/>
       <c r="H63" s="25"/>
       <c r="I63" s="23"/>
       <c r="J63" s="26"/>
-      <c r="K63" s="48" t="s">
+      <c r="K63" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2598,15 +2599,15 @@
         <v>54</v>
       </c>
       <c r="B64" s="27"/>
-      <c r="C64" s="51"/>
-      <c r="D64" s="51"/>
+      <c r="C64" s="50"/>
+      <c r="D64" s="50"/>
       <c r="E64" s="24"/>
-      <c r="F64" s="43"/>
-      <c r="G64" s="43"/>
+      <c r="F64" s="42"/>
+      <c r="G64" s="42"/>
       <c r="H64" s="25"/>
       <c r="I64" s="23"/>
       <c r="J64" s="26"/>
-      <c r="K64" s="48" t="s">
+      <c r="K64" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2615,15 +2616,15 @@
         <v>55</v>
       </c>
       <c r="B65" s="27"/>
-      <c r="C65" s="51"/>
-      <c r="D65" s="51"/>
+      <c r="C65" s="50"/>
+      <c r="D65" s="50"/>
       <c r="E65" s="24"/>
-      <c r="F65" s="43"/>
-      <c r="G65" s="43"/>
+      <c r="F65" s="42"/>
+      <c r="G65" s="42"/>
       <c r="H65" s="25"/>
       <c r="I65" s="23"/>
       <c r="J65" s="26"/>
-      <c r="K65" s="48" t="s">
+      <c r="K65" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2632,15 +2633,15 @@
         <v>56</v>
       </c>
       <c r="B66" s="27"/>
-      <c r="C66" s="51"/>
-      <c r="D66" s="51"/>
+      <c r="C66" s="50"/>
+      <c r="D66" s="50"/>
       <c r="E66" s="24"/>
-      <c r="F66" s="43"/>
-      <c r="G66" s="43"/>
+      <c r="F66" s="42"/>
+      <c r="G66" s="42"/>
       <c r="H66" s="25"/>
       <c r="I66" s="23"/>
       <c r="J66" s="26"/>
-      <c r="K66" s="48" t="s">
+      <c r="K66" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2649,15 +2650,15 @@
         <v>57</v>
       </c>
       <c r="B67" s="27"/>
-      <c r="C67" s="51"/>
-      <c r="D67" s="51"/>
+      <c r="C67" s="50"/>
+      <c r="D67" s="50"/>
       <c r="E67" s="24"/>
-      <c r="F67" s="43"/>
-      <c r="G67" s="43"/>
+      <c r="F67" s="42"/>
+      <c r="G67" s="42"/>
       <c r="H67" s="25"/>
       <c r="I67" s="23"/>
       <c r="J67" s="26"/>
-      <c r="K67" s="48" t="s">
+      <c r="K67" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2666,15 +2667,15 @@
         <v>58</v>
       </c>
       <c r="B68" s="27"/>
-      <c r="C68" s="51"/>
-      <c r="D68" s="51"/>
+      <c r="C68" s="50"/>
+      <c r="D68" s="50"/>
       <c r="E68" s="24"/>
-      <c r="F68" s="43"/>
-      <c r="G68" s="43"/>
+      <c r="F68" s="42"/>
+      <c r="G68" s="42"/>
       <c r="H68" s="25"/>
       <c r="I68" s="23"/>
       <c r="J68" s="26"/>
-      <c r="K68" s="48" t="s">
+      <c r="K68" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2683,15 +2684,15 @@
         <v>59</v>
       </c>
       <c r="B69" s="27"/>
-      <c r="C69" s="51"/>
-      <c r="D69" s="51"/>
+      <c r="C69" s="50"/>
+      <c r="D69" s="50"/>
       <c r="E69" s="24"/>
-      <c r="F69" s="43"/>
-      <c r="G69" s="43"/>
+      <c r="F69" s="42"/>
+      <c r="G69" s="42"/>
       <c r="H69" s="25"/>
       <c r="I69" s="23"/>
       <c r="J69" s="26"/>
-      <c r="K69" s="48" t="s">
+      <c r="K69" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2700,70 +2701,63 @@
         <v>60</v>
       </c>
       <c r="B70" s="30"/>
-      <c r="C70" s="53"/>
-      <c r="D70" s="54"/>
+      <c r="C70" s="52"/>
+      <c r="D70" s="53"/>
       <c r="E70" s="31"/>
-      <c r="F70" s="43"/>
-      <c r="G70" s="43"/>
+      <c r="F70" s="42"/>
+      <c r="G70" s="42"/>
       <c r="H70" s="32"/>
       <c r="I70" s="33"/>
       <c r="J70" s="34"/>
-      <c r="K70" s="55" t="s">
+      <c r="K70" s="54" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="71" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="63" t="s">
+      <c r="A71" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="B71" s="63"/>
-      <c r="C71" s="63"/>
-      <c r="D71" s="35"/>
-      <c r="E71" s="36"/>
-      <c r="F71" s="36"/>
-      <c r="G71" s="36"/>
+      <c r="B71" s="69"/>
+      <c r="C71" s="69"/>
+      <c r="D71" s="90"/>
+      <c r="E71" s="35"/>
+      <c r="F71" s="35"/>
+      <c r="G71" s="35"/>
       <c r="H71" s="2"/>
       <c r="I71" s="2"/>
       <c r="J71" s="2"/>
     </row>
     <row r="72" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D72" s="37" t="s">
+      <c r="D72" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="E72" s="37"/>
-      <c r="F72" s="37"/>
-      <c r="G72" s="37"/>
+      <c r="E72" s="36"/>
+      <c r="F72" s="36"/>
+      <c r="G72" s="36"/>
     </row>
     <row r="73" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G73" s="38"/>
-      <c r="H73" s="38"/>
-      <c r="I73" s="38"/>
-      <c r="J73" s="38"/>
+      <c r="G73" s="37"/>
+      <c r="H73" s="37"/>
+      <c r="I73" s="37"/>
+      <c r="J73" s="37"/>
     </row>
     <row r="74" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="39" t="s">
+      <c r="A74" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="C74" s="64"/>
-      <c r="D74" s="64"/>
+      <c r="C74" s="70"/>
+      <c r="D74" s="70"/>
       <c r="E74" s="4"/>
       <c r="F74" s="4"/>
-      <c r="G74" s="65" t="s">
+      <c r="G74" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="H74" s="65"/>
-      <c r="I74" s="65"/>
-      <c r="J74" s="65"/>
+      <c r="H74" s="71"/>
+      <c r="I74" s="71"/>
+      <c r="J74" s="71"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="I5:J5"/>
     <mergeCell ref="A71:C71"/>
     <mergeCell ref="C74:D74"/>
     <mergeCell ref="G74:J74"/>
@@ -2778,6 +2772,13 @@
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="F9:G9"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="I5:J5"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="70" fitToHeight="0" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2808,156 +2809,156 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="57"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="58" t="s">
+      <c r="A2" s="56"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="88" t="s">
+      <c r="D2" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
-      <c r="L2" s="57"/>
-      <c r="M2" s="57"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
     </row>
     <row r="3" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="89" t="s">
+      <c r="A3" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="89"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60"/>
-      <c r="M3" s="59"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
+      <c r="J3" s="66"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="58"/>
     </row>
     <row r="4" spans="1:13" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J4" s="62"/>
+      <c r="J4" s="61"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="90"/>
-      <c r="D5" s="90"/>
-      <c r="E5" s="90"/>
-      <c r="F5" s="90"/>
-      <c r="G5" s="90"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
       <c r="H5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="67" t="s">
+      <c r="I5" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="J5" s="67"/>
+      <c r="J5" s="68"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="66"/>
-      <c r="D6" s="66"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="66"/>
-      <c r="G6" s="66"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="62"/>
       <c r="H6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="86"/>
-      <c r="J6" s="86"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="63"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="66"/>
-      <c r="D7" s="66"/>
-      <c r="E7" s="66"/>
-      <c r="F7" s="66"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
       <c r="G7" s="6"/>
       <c r="H7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="67"/>
-      <c r="J7" s="67"/>
+      <c r="I7" s="68"/>
+      <c r="J7" s="68"/>
     </row>
     <row r="8" spans="1:13" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J8" s="40"/>
+      <c r="J8" s="39"/>
     </row>
     <row r="9" spans="1:13" s="8" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="68" t="s">
+      <c r="A9" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="70" t="s">
+      <c r="B9" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="72" t="s">
+      <c r="C9" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="74" t="s">
+      <c r="D9" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="76" t="s">
+      <c r="E9" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="84" t="s">
+      <c r="F9" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="85"/>
-      <c r="H9" s="78" t="s">
+      <c r="G9" s="89"/>
+      <c r="H9" s="82" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="80" t="s">
+      <c r="I9" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="J9" s="82" t="s">
+      <c r="J9" s="86" t="s">
         <v>17</v>
       </c>
-      <c r="K9" s="83"/>
+      <c r="K9" s="87"/>
     </row>
     <row r="10" spans="1:13" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="69"/>
-      <c r="B10" s="71"/>
-      <c r="C10" s="73"/>
-      <c r="D10" s="75"/>
-      <c r="E10" s="77"/>
-      <c r="F10" s="44" t="s">
+      <c r="A10" s="73"/>
+      <c r="B10" s="75"/>
+      <c r="C10" s="77"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="81"/>
+      <c r="F10" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="G10" s="42" t="s">
+      <c r="G10" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="H10" s="79"/>
-      <c r="I10" s="81"/>
+      <c r="H10" s="83"/>
+      <c r="I10" s="85"/>
       <c r="J10" s="9" t="s">
         <v>18</v>
       </c>
@@ -2973,12 +2974,12 @@
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
       <c r="E11" s="14"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
       <c r="H11" s="15"/>
-      <c r="I11" s="47"/>
+      <c r="I11" s="46"/>
       <c r="J11" s="16"/>
-      <c r="K11" s="48" t="s">
+      <c r="K11" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2990,12 +2991,12 @@
       <c r="C12" s="19"/>
       <c r="D12" s="19"/>
       <c r="E12" s="20"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
       <c r="H12" s="21"/>
-      <c r="I12" s="49"/>
+      <c r="I12" s="48"/>
       <c r="J12" s="22"/>
-      <c r="K12" s="48" t="s">
+      <c r="K12" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3007,12 +3008,12 @@
       <c r="C13" s="19"/>
       <c r="D13" s="19"/>
       <c r="E13" s="20"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
       <c r="H13" s="21"/>
-      <c r="I13" s="49"/>
+      <c r="I13" s="48"/>
       <c r="J13" s="22"/>
-      <c r="K13" s="48" t="s">
+      <c r="K13" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3024,12 +3025,12 @@
       <c r="C14" s="19"/>
       <c r="D14" s="19"/>
       <c r="E14" s="20"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
       <c r="H14" s="21"/>
-      <c r="I14" s="49"/>
+      <c r="I14" s="48"/>
       <c r="J14" s="22"/>
-      <c r="K14" s="48" t="s">
+      <c r="K14" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3041,12 +3042,12 @@
       <c r="C15" s="19"/>
       <c r="D15" s="19"/>
       <c r="E15" s="20"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="43"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="42"/>
       <c r="H15" s="21"/>
-      <c r="I15" s="49"/>
+      <c r="I15" s="48"/>
       <c r="J15" s="22"/>
-      <c r="K15" s="48" t="s">
+      <c r="K15" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3058,12 +3059,12 @@
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
       <c r="E16" s="20"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="43"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
       <c r="H16" s="21"/>
       <c r="I16" s="23"/>
       <c r="J16" s="22"/>
-      <c r="K16" s="48" t="s">
+      <c r="K16" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3075,12 +3076,12 @@
       <c r="C17" s="19"/>
       <c r="D17" s="19"/>
       <c r="E17" s="20"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="43"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
       <c r="H17" s="21"/>
       <c r="I17" s="23"/>
       <c r="J17" s="22"/>
-      <c r="K17" s="48" t="s">
+      <c r="K17" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3092,12 +3093,12 @@
       <c r="C18" s="19"/>
       <c r="D18" s="19"/>
       <c r="E18" s="20"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
       <c r="H18" s="21"/>
-      <c r="I18" s="49"/>
+      <c r="I18" s="48"/>
       <c r="J18" s="22"/>
-      <c r="K18" s="48" t="s">
+      <c r="K18" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3109,12 +3110,12 @@
       <c r="C19" s="19"/>
       <c r="D19" s="19"/>
       <c r="E19" s="20"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="42"/>
       <c r="H19" s="21"/>
-      <c r="I19" s="49"/>
+      <c r="I19" s="48"/>
       <c r="J19" s="22"/>
-      <c r="K19" s="48" t="s">
+      <c r="K19" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3126,12 +3127,12 @@
       <c r="C20" s="19"/>
       <c r="D20" s="19"/>
       <c r="E20" s="20"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="43"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="42"/>
       <c r="H20" s="21"/>
-      <c r="I20" s="49"/>
+      <c r="I20" s="48"/>
       <c r="J20" s="22"/>
-      <c r="K20" s="48" t="s">
+      <c r="K20" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3143,12 +3144,12 @@
       <c r="C21" s="19"/>
       <c r="D21" s="19"/>
       <c r="E21" s="20"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="43"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="42"/>
       <c r="H21" s="21"/>
-      <c r="I21" s="49"/>
+      <c r="I21" s="48"/>
       <c r="J21" s="22"/>
-      <c r="K21" s="48" t="s">
+      <c r="K21" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3160,12 +3161,12 @@
       <c r="C22" s="19"/>
       <c r="D22" s="19"/>
       <c r="E22" s="20"/>
-      <c r="F22" s="43"/>
-      <c r="G22" s="43"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="42"/>
       <c r="H22" s="21"/>
-      <c r="I22" s="49"/>
+      <c r="I22" s="48"/>
       <c r="J22" s="22"/>
-      <c r="K22" s="48" t="s">
+      <c r="K22" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3177,12 +3178,12 @@
       <c r="C23" s="19"/>
       <c r="D23" s="19"/>
       <c r="E23" s="20"/>
-      <c r="F23" s="43"/>
-      <c r="G23" s="43"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="42"/>
       <c r="H23" s="21"/>
-      <c r="I23" s="49"/>
+      <c r="I23" s="48"/>
       <c r="J23" s="22"/>
-      <c r="K23" s="48" t="s">
+      <c r="K23" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3190,16 +3191,16 @@
       <c r="A24" s="17">
         <v>74</v>
       </c>
-      <c r="B24" s="50"/>
-      <c r="C24" s="51"/>
-      <c r="D24" s="51"/>
+      <c r="B24" s="49"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="50"/>
       <c r="E24" s="20"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="43"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="42"/>
       <c r="H24" s="21"/>
-      <c r="I24" s="49"/>
-      <c r="J24" s="52"/>
-      <c r="K24" s="48" t="s">
+      <c r="I24" s="48"/>
+      <c r="J24" s="51"/>
+      <c r="K24" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3207,16 +3208,16 @@
       <c r="A25" s="11">
         <v>75</v>
       </c>
-      <c r="B25" s="50"/>
-      <c r="C25" s="51"/>
-      <c r="D25" s="51"/>
+      <c r="B25" s="49"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="50"/>
       <c r="E25" s="20"/>
-      <c r="F25" s="43"/>
-      <c r="G25" s="43"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="42"/>
       <c r="H25" s="21"/>
-      <c r="I25" s="49"/>
-      <c r="J25" s="52"/>
-      <c r="K25" s="48" t="s">
+      <c r="I25" s="48"/>
+      <c r="J25" s="51"/>
+      <c r="K25" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3224,16 +3225,16 @@
       <c r="A26" s="17">
         <v>76</v>
       </c>
-      <c r="B26" s="50"/>
-      <c r="C26" s="51"/>
-      <c r="D26" s="51"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="50"/>
       <c r="E26" s="24"/>
-      <c r="F26" s="43"/>
-      <c r="G26" s="43"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="42"/>
       <c r="H26" s="25"/>
       <c r="I26" s="23"/>
       <c r="J26" s="26"/>
-      <c r="K26" s="48" t="s">
+      <c r="K26" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3241,16 +3242,16 @@
       <c r="A27" s="11">
         <v>77</v>
       </c>
-      <c r="B27" s="50"/>
-      <c r="C27" s="51"/>
-      <c r="D27" s="51"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="50"/>
+      <c r="D27" s="50"/>
       <c r="E27" s="20"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="43"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
       <c r="H27" s="21"/>
-      <c r="I27" s="49"/>
-      <c r="J27" s="52"/>
-      <c r="K27" s="48" t="s">
+      <c r="I27" s="48"/>
+      <c r="J27" s="51"/>
+      <c r="K27" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3258,16 +3259,16 @@
       <c r="A28" s="17">
         <v>78</v>
       </c>
-      <c r="B28" s="50"/>
-      <c r="C28" s="51"/>
-      <c r="D28" s="51"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="50"/>
       <c r="E28" s="24"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
+      <c r="F28" s="42"/>
+      <c r="G28" s="42"/>
       <c r="H28" s="25"/>
       <c r="I28" s="23"/>
       <c r="J28" s="26"/>
-      <c r="K28" s="48" t="s">
+      <c r="K28" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3275,16 +3276,16 @@
       <c r="A29" s="11">
         <v>79</v>
       </c>
-      <c r="B29" s="50"/>
-      <c r="C29" s="51"/>
-      <c r="D29" s="51"/>
+      <c r="B29" s="49"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="50"/>
       <c r="E29" s="24"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="43"/>
+      <c r="F29" s="42"/>
+      <c r="G29" s="42"/>
       <c r="H29" s="25"/>
       <c r="I29" s="23"/>
       <c r="J29" s="26"/>
-      <c r="K29" s="48" t="s">
+      <c r="K29" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3292,16 +3293,16 @@
       <c r="A30" s="17">
         <v>80</v>
       </c>
-      <c r="B30" s="50"/>
-      <c r="C30" s="51"/>
-      <c r="D30" s="51"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="50"/>
+      <c r="D30" s="50"/>
       <c r="E30" s="24"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="43"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="42"/>
       <c r="H30" s="25"/>
       <c r="I30" s="23"/>
       <c r="J30" s="26"/>
-      <c r="K30" s="48" t="s">
+      <c r="K30" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3309,16 +3310,16 @@
       <c r="A31" s="11">
         <v>81</v>
       </c>
-      <c r="B31" s="50"/>
-      <c r="C31" s="51"/>
-      <c r="D31" s="51"/>
+      <c r="B31" s="49"/>
+      <c r="C31" s="50"/>
+      <c r="D31" s="50"/>
       <c r="E31" s="24"/>
-      <c r="F31" s="43"/>
-      <c r="G31" s="43"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="42"/>
       <c r="H31" s="25"/>
       <c r="I31" s="23"/>
       <c r="J31" s="26"/>
-      <c r="K31" s="48" t="s">
+      <c r="K31" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3326,16 +3327,16 @@
       <c r="A32" s="17">
         <v>82</v>
       </c>
-      <c r="B32" s="50"/>
-      <c r="C32" s="51"/>
-      <c r="D32" s="51"/>
+      <c r="B32" s="49"/>
+      <c r="C32" s="50"/>
+      <c r="D32" s="50"/>
       <c r="E32" s="20"/>
-      <c r="F32" s="43"/>
-      <c r="G32" s="43"/>
+      <c r="F32" s="42"/>
+      <c r="G32" s="42"/>
       <c r="H32" s="21"/>
-      <c r="I32" s="49"/>
-      <c r="J32" s="52"/>
-      <c r="K32" s="48" t="s">
+      <c r="I32" s="48"/>
+      <c r="J32" s="51"/>
+      <c r="K32" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3343,16 +3344,16 @@
       <c r="A33" s="11">
         <v>83</v>
       </c>
-      <c r="B33" s="50"/>
-      <c r="C33" s="51"/>
-      <c r="D33" s="51"/>
+      <c r="B33" s="49"/>
+      <c r="C33" s="50"/>
+      <c r="D33" s="50"/>
       <c r="E33" s="20"/>
-      <c r="F33" s="43"/>
-      <c r="G33" s="43"/>
+      <c r="F33" s="42"/>
+      <c r="G33" s="42"/>
       <c r="H33" s="21"/>
-      <c r="I33" s="49"/>
-      <c r="J33" s="52"/>
-      <c r="K33" s="48" t="s">
+      <c r="I33" s="48"/>
+      <c r="J33" s="51"/>
+      <c r="K33" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3360,16 +3361,16 @@
       <c r="A34" s="17">
         <v>84</v>
       </c>
-      <c r="B34" s="50"/>
-      <c r="C34" s="51"/>
-      <c r="D34" s="51"/>
+      <c r="B34" s="49"/>
+      <c r="C34" s="50"/>
+      <c r="D34" s="50"/>
       <c r="E34" s="24"/>
-      <c r="F34" s="43"/>
-      <c r="G34" s="43"/>
+      <c r="F34" s="42"/>
+      <c r="G34" s="42"/>
       <c r="H34" s="25"/>
       <c r="I34" s="23"/>
       <c r="J34" s="26"/>
-      <c r="K34" s="48" t="s">
+      <c r="K34" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3377,16 +3378,16 @@
       <c r="A35" s="11">
         <v>85</v>
       </c>
-      <c r="B35" s="50"/>
-      <c r="C35" s="51"/>
-      <c r="D35" s="51"/>
+      <c r="B35" s="49"/>
+      <c r="C35" s="50"/>
+      <c r="D35" s="50"/>
       <c r="E35" s="20"/>
-      <c r="F35" s="43"/>
-      <c r="G35" s="43"/>
+      <c r="F35" s="42"/>
+      <c r="G35" s="42"/>
       <c r="H35" s="21"/>
-      <c r="I35" s="49"/>
-      <c r="J35" s="52"/>
-      <c r="K35" s="48" t="s">
+      <c r="I35" s="48"/>
+      <c r="J35" s="51"/>
+      <c r="K35" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3394,16 +3395,16 @@
       <c r="A36" s="17">
         <v>86</v>
       </c>
-      <c r="B36" s="50"/>
-      <c r="C36" s="51"/>
-      <c r="D36" s="51"/>
+      <c r="B36" s="49"/>
+      <c r="C36" s="50"/>
+      <c r="D36" s="50"/>
       <c r="E36" s="24"/>
-      <c r="F36" s="43"/>
-      <c r="G36" s="43"/>
+      <c r="F36" s="42"/>
+      <c r="G36" s="42"/>
       <c r="H36" s="25"/>
       <c r="I36" s="23"/>
       <c r="J36" s="26"/>
-      <c r="K36" s="48" t="s">
+      <c r="K36" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3411,16 +3412,16 @@
       <c r="A37" s="11">
         <v>87</v>
       </c>
-      <c r="B37" s="50"/>
-      <c r="C37" s="51"/>
-      <c r="D37" s="51"/>
+      <c r="B37" s="49"/>
+      <c r="C37" s="50"/>
+      <c r="D37" s="50"/>
       <c r="E37" s="24"/>
-      <c r="F37" s="43"/>
-      <c r="G37" s="43"/>
+      <c r="F37" s="42"/>
+      <c r="G37" s="42"/>
       <c r="H37" s="25"/>
       <c r="I37" s="23"/>
       <c r="J37" s="26"/>
-      <c r="K37" s="48" t="s">
+      <c r="K37" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3428,16 +3429,16 @@
       <c r="A38" s="17">
         <v>88</v>
       </c>
-      <c r="B38" s="50"/>
-      <c r="C38" s="51"/>
-      <c r="D38" s="51"/>
+      <c r="B38" s="49"/>
+      <c r="C38" s="50"/>
+      <c r="D38" s="50"/>
       <c r="E38" s="24"/>
-      <c r="F38" s="43"/>
-      <c r="G38" s="43"/>
+      <c r="F38" s="42"/>
+      <c r="G38" s="42"/>
       <c r="H38" s="25"/>
       <c r="I38" s="23"/>
       <c r="J38" s="26"/>
-      <c r="K38" s="48" t="s">
+      <c r="K38" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3445,16 +3446,16 @@
       <c r="A39" s="11">
         <v>89</v>
       </c>
-      <c r="B39" s="50"/>
-      <c r="C39" s="51"/>
-      <c r="D39" s="51"/>
+      <c r="B39" s="49"/>
+      <c r="C39" s="50"/>
+      <c r="D39" s="50"/>
       <c r="E39" s="20"/>
-      <c r="F39" s="43"/>
-      <c r="G39" s="43"/>
+      <c r="F39" s="42"/>
+      <c r="G39" s="42"/>
       <c r="H39" s="21"/>
-      <c r="I39" s="49"/>
-      <c r="J39" s="52"/>
-      <c r="K39" s="48" t="s">
+      <c r="I39" s="48"/>
+      <c r="J39" s="51"/>
+      <c r="K39" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3462,16 +3463,16 @@
       <c r="A40" s="17">
         <v>90</v>
       </c>
-      <c r="B40" s="50"/>
-      <c r="C40" s="51"/>
-      <c r="D40" s="51"/>
+      <c r="B40" s="49"/>
+      <c r="C40" s="50"/>
+      <c r="D40" s="50"/>
       <c r="E40" s="20"/>
-      <c r="F40" s="43"/>
-      <c r="G40" s="43"/>
+      <c r="F40" s="42"/>
+      <c r="G40" s="42"/>
       <c r="H40" s="21"/>
-      <c r="I40" s="49"/>
-      <c r="J40" s="52"/>
-      <c r="K40" s="48" t="s">
+      <c r="I40" s="48"/>
+      <c r="J40" s="51"/>
+      <c r="K40" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3479,16 +3480,16 @@
       <c r="A41" s="11">
         <v>91</v>
       </c>
-      <c r="B41" s="50"/>
-      <c r="C41" s="51"/>
-      <c r="D41" s="51"/>
+      <c r="B41" s="49"/>
+      <c r="C41" s="50"/>
+      <c r="D41" s="50"/>
       <c r="E41" s="20"/>
-      <c r="F41" s="43"/>
-      <c r="G41" s="43"/>
+      <c r="F41" s="42"/>
+      <c r="G41" s="42"/>
       <c r="H41" s="21"/>
-      <c r="I41" s="49"/>
-      <c r="J41" s="52"/>
-      <c r="K41" s="48" t="s">
+      <c r="I41" s="48"/>
+      <c r="J41" s="51"/>
+      <c r="K41" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3496,16 +3497,16 @@
       <c r="A42" s="17">
         <v>92</v>
       </c>
-      <c r="B42" s="50"/>
-      <c r="C42" s="51"/>
-      <c r="D42" s="51"/>
+      <c r="B42" s="49"/>
+      <c r="C42" s="50"/>
+      <c r="D42" s="50"/>
       <c r="E42" s="24"/>
-      <c r="F42" s="43"/>
-      <c r="G42" s="43"/>
+      <c r="F42" s="42"/>
+      <c r="G42" s="42"/>
       <c r="H42" s="25"/>
       <c r="I42" s="23"/>
       <c r="J42" s="26"/>
-      <c r="K42" s="48" t="s">
+      <c r="K42" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3513,16 +3514,16 @@
       <c r="A43" s="11">
         <v>93</v>
       </c>
-      <c r="B43" s="50"/>
-      <c r="C43" s="51"/>
-      <c r="D43" s="51"/>
+      <c r="B43" s="49"/>
+      <c r="C43" s="50"/>
+      <c r="D43" s="50"/>
       <c r="E43" s="20"/>
-      <c r="F43" s="43"/>
-      <c r="G43" s="43"/>
+      <c r="F43" s="42"/>
+      <c r="G43" s="42"/>
       <c r="H43" s="21"/>
-      <c r="I43" s="49"/>
-      <c r="J43" s="52"/>
-      <c r="K43" s="48" t="s">
+      <c r="I43" s="48"/>
+      <c r="J43" s="51"/>
+      <c r="K43" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3530,16 +3531,16 @@
       <c r="A44" s="17">
         <v>94</v>
       </c>
-      <c r="B44" s="50"/>
-      <c r="C44" s="51"/>
-      <c r="D44" s="51"/>
+      <c r="B44" s="49"/>
+      <c r="C44" s="50"/>
+      <c r="D44" s="50"/>
       <c r="E44" s="24"/>
-      <c r="F44" s="43"/>
-      <c r="G44" s="43"/>
+      <c r="F44" s="42"/>
+      <c r="G44" s="42"/>
       <c r="H44" s="25"/>
       <c r="I44" s="23"/>
       <c r="J44" s="26"/>
-      <c r="K44" s="48" t="s">
+      <c r="K44" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3547,16 +3548,16 @@
       <c r="A45" s="11">
         <v>95</v>
       </c>
-      <c r="B45" s="50"/>
-      <c r="C45" s="51"/>
-      <c r="D45" s="51"/>
+      <c r="B45" s="49"/>
+      <c r="C45" s="50"/>
+      <c r="D45" s="50"/>
       <c r="E45" s="20"/>
-      <c r="F45" s="43"/>
-      <c r="G45" s="43"/>
+      <c r="F45" s="42"/>
+      <c r="G45" s="42"/>
       <c r="H45" s="21"/>
-      <c r="I45" s="49"/>
-      <c r="J45" s="52"/>
-      <c r="K45" s="48" t="s">
+      <c r="I45" s="48"/>
+      <c r="J45" s="51"/>
+      <c r="K45" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3565,15 +3566,15 @@
         <v>96</v>
       </c>
       <c r="B46" s="27"/>
-      <c r="C46" s="51"/>
-      <c r="D46" s="51"/>
+      <c r="C46" s="50"/>
+      <c r="D46" s="50"/>
       <c r="E46" s="24"/>
-      <c r="F46" s="43"/>
-      <c r="G46" s="43"/>
+      <c r="F46" s="42"/>
+      <c r="G46" s="42"/>
       <c r="H46" s="25"/>
       <c r="I46" s="23"/>
       <c r="J46" s="26"/>
-      <c r="K46" s="48" t="s">
+      <c r="K46" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3582,15 +3583,15 @@
         <v>97</v>
       </c>
       <c r="B47" s="27"/>
-      <c r="C47" s="51"/>
-      <c r="D47" s="51"/>
+      <c r="C47" s="50"/>
+      <c r="D47" s="50"/>
       <c r="E47" s="24"/>
-      <c r="F47" s="43"/>
-      <c r="G47" s="43"/>
+      <c r="F47" s="42"/>
+      <c r="G47" s="42"/>
       <c r="H47" s="25"/>
       <c r="I47" s="23"/>
       <c r="J47" s="26"/>
-      <c r="K47" s="48" t="s">
+      <c r="K47" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3599,15 +3600,15 @@
         <v>98</v>
       </c>
       <c r="B48" s="27"/>
-      <c r="C48" s="51"/>
-      <c r="D48" s="51"/>
+      <c r="C48" s="50"/>
+      <c r="D48" s="50"/>
       <c r="E48" s="24"/>
-      <c r="F48" s="43"/>
-      <c r="G48" s="43"/>
+      <c r="F48" s="42"/>
+      <c r="G48" s="42"/>
       <c r="H48" s="25"/>
       <c r="I48" s="23"/>
       <c r="J48" s="26"/>
-      <c r="K48" s="48" t="s">
+      <c r="K48" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3616,15 +3617,15 @@
         <v>99</v>
       </c>
       <c r="B49" s="27"/>
-      <c r="C49" s="51"/>
-      <c r="D49" s="51"/>
+      <c r="C49" s="50"/>
+      <c r="D49" s="50"/>
       <c r="E49" s="24"/>
-      <c r="F49" s="43"/>
-      <c r="G49" s="43"/>
+      <c r="F49" s="42"/>
+      <c r="G49" s="42"/>
       <c r="H49" s="25"/>
       <c r="I49" s="23"/>
       <c r="J49" s="26"/>
-      <c r="K49" s="48" t="s">
+      <c r="K49" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3633,15 +3634,15 @@
         <v>100</v>
       </c>
       <c r="B50" s="27"/>
-      <c r="C50" s="51"/>
-      <c r="D50" s="51"/>
+      <c r="C50" s="50"/>
+      <c r="D50" s="50"/>
       <c r="E50" s="24"/>
-      <c r="F50" s="43"/>
-      <c r="G50" s="43"/>
+      <c r="F50" s="42"/>
+      <c r="G50" s="42"/>
       <c r="H50" s="25"/>
       <c r="I50" s="23"/>
       <c r="J50" s="26"/>
-      <c r="K50" s="48" t="s">
+      <c r="K50" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3650,15 +3651,15 @@
         <v>101</v>
       </c>
       <c r="B51" s="27"/>
-      <c r="C51" s="51"/>
-      <c r="D51" s="51"/>
+      <c r="C51" s="50"/>
+      <c r="D51" s="50"/>
       <c r="E51" s="24"/>
-      <c r="F51" s="43"/>
-      <c r="G51" s="43"/>
+      <c r="F51" s="42"/>
+      <c r="G51" s="42"/>
       <c r="H51" s="25"/>
       <c r="I51" s="23"/>
       <c r="J51" s="26"/>
-      <c r="K51" s="48" t="s">
+      <c r="K51" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3667,15 +3668,15 @@
         <v>102</v>
       </c>
       <c r="B52" s="27"/>
-      <c r="C52" s="51"/>
-      <c r="D52" s="51"/>
+      <c r="C52" s="50"/>
+      <c r="D52" s="50"/>
       <c r="E52" s="24"/>
-      <c r="F52" s="43"/>
-      <c r="G52" s="43"/>
+      <c r="F52" s="42"/>
+      <c r="G52" s="42"/>
       <c r="H52" s="25"/>
       <c r="I52" s="23"/>
       <c r="J52" s="26"/>
-      <c r="K52" s="48" t="s">
+      <c r="K52" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3684,15 +3685,15 @@
         <v>103</v>
       </c>
       <c r="B53" s="27"/>
-      <c r="C53" s="51"/>
-      <c r="D53" s="51"/>
+      <c r="C53" s="50"/>
+      <c r="D53" s="50"/>
       <c r="E53" s="24"/>
-      <c r="F53" s="43"/>
-      <c r="G53" s="43"/>
+      <c r="F53" s="42"/>
+      <c r="G53" s="42"/>
       <c r="H53" s="25"/>
       <c r="I53" s="23"/>
       <c r="J53" s="26"/>
-      <c r="K53" s="48" t="s">
+      <c r="K53" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3701,15 +3702,15 @@
         <v>104</v>
       </c>
       <c r="B54" s="27"/>
-      <c r="C54" s="51"/>
-      <c r="D54" s="51"/>
+      <c r="C54" s="50"/>
+      <c r="D54" s="50"/>
       <c r="E54" s="24"/>
-      <c r="F54" s="43"/>
-      <c r="G54" s="43"/>
+      <c r="F54" s="42"/>
+      <c r="G54" s="42"/>
       <c r="H54" s="25"/>
       <c r="I54" s="23"/>
       <c r="J54" s="26"/>
-      <c r="K54" s="48" t="s">
+      <c r="K54" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3718,15 +3719,15 @@
         <v>105</v>
       </c>
       <c r="B55" s="27"/>
-      <c r="C55" s="51"/>
-      <c r="D55" s="51"/>
+      <c r="C55" s="50"/>
+      <c r="D55" s="50"/>
       <c r="E55" s="24"/>
-      <c r="F55" s="43"/>
-      <c r="G55" s="43"/>
+      <c r="F55" s="42"/>
+      <c r="G55" s="42"/>
       <c r="H55" s="25"/>
       <c r="I55" s="23"/>
       <c r="J55" s="26"/>
-      <c r="K55" s="48" t="s">
+      <c r="K55" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3735,15 +3736,15 @@
         <v>106</v>
       </c>
       <c r="B56" s="27"/>
-      <c r="C56" s="51"/>
-      <c r="D56" s="51"/>
+      <c r="C56" s="50"/>
+      <c r="D56" s="50"/>
       <c r="E56" s="24"/>
-      <c r="F56" s="43"/>
-      <c r="G56" s="43"/>
+      <c r="F56" s="42"/>
+      <c r="G56" s="42"/>
       <c r="H56" s="25"/>
       <c r="I56" s="23"/>
       <c r="J56" s="26"/>
-      <c r="K56" s="48" t="s">
+      <c r="K56" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3752,15 +3753,15 @@
         <v>107</v>
       </c>
       <c r="B57" s="27"/>
-      <c r="C57" s="51"/>
-      <c r="D57" s="51"/>
+      <c r="C57" s="50"/>
+      <c r="D57" s="50"/>
       <c r="E57" s="24"/>
-      <c r="F57" s="43"/>
-      <c r="G57" s="43"/>
+      <c r="F57" s="42"/>
+      <c r="G57" s="42"/>
       <c r="H57" s="25"/>
       <c r="I57" s="23"/>
       <c r="J57" s="26"/>
-      <c r="K57" s="48" t="s">
+      <c r="K57" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3769,15 +3770,15 @@
         <v>108</v>
       </c>
       <c r="B58" s="27"/>
-      <c r="C58" s="51"/>
-      <c r="D58" s="51"/>
+      <c r="C58" s="50"/>
+      <c r="D58" s="50"/>
       <c r="E58" s="24"/>
-      <c r="F58" s="43"/>
-      <c r="G58" s="43"/>
+      <c r="F58" s="42"/>
+      <c r="G58" s="42"/>
       <c r="H58" s="25"/>
       <c r="I58" s="23"/>
       <c r="J58" s="26"/>
-      <c r="K58" s="48" t="s">
+      <c r="K58" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3786,15 +3787,15 @@
         <v>109</v>
       </c>
       <c r="B59" s="27"/>
-      <c r="C59" s="51"/>
-      <c r="D59" s="51"/>
+      <c r="C59" s="50"/>
+      <c r="D59" s="50"/>
       <c r="E59" s="24"/>
-      <c r="F59" s="43"/>
-      <c r="G59" s="43"/>
+      <c r="F59" s="42"/>
+      <c r="G59" s="42"/>
       <c r="H59" s="25"/>
       <c r="I59" s="23"/>
       <c r="J59" s="26"/>
-      <c r="K59" s="48" t="s">
+      <c r="K59" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3803,15 +3804,15 @@
         <v>110</v>
       </c>
       <c r="B60" s="27"/>
-      <c r="C60" s="51"/>
-      <c r="D60" s="51"/>
+      <c r="C60" s="50"/>
+      <c r="D60" s="50"/>
       <c r="E60" s="24"/>
-      <c r="F60" s="43"/>
-      <c r="G60" s="43"/>
+      <c r="F60" s="42"/>
+      <c r="G60" s="42"/>
       <c r="H60" s="25"/>
       <c r="I60" s="23"/>
       <c r="J60" s="26"/>
-      <c r="K60" s="48" t="s">
+      <c r="K60" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3820,15 +3821,15 @@
         <v>111</v>
       </c>
       <c r="B61" s="27"/>
-      <c r="C61" s="51"/>
-      <c r="D61" s="51"/>
+      <c r="C61" s="50"/>
+      <c r="D61" s="50"/>
       <c r="E61" s="24"/>
-      <c r="F61" s="43"/>
-      <c r="G61" s="43"/>
+      <c r="F61" s="42"/>
+      <c r="G61" s="42"/>
       <c r="H61" s="25"/>
       <c r="I61" s="23"/>
       <c r="J61" s="26"/>
-      <c r="K61" s="48" t="s">
+      <c r="K61" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3837,15 +3838,15 @@
         <v>112</v>
       </c>
       <c r="B62" s="27"/>
-      <c r="C62" s="51"/>
-      <c r="D62" s="51"/>
+      <c r="C62" s="50"/>
+      <c r="D62" s="50"/>
       <c r="E62" s="24"/>
-      <c r="F62" s="43"/>
-      <c r="G62" s="43"/>
+      <c r="F62" s="42"/>
+      <c r="G62" s="42"/>
       <c r="H62" s="25"/>
       <c r="I62" s="23"/>
       <c r="J62" s="26"/>
-      <c r="K62" s="48" t="s">
+      <c r="K62" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3854,15 +3855,15 @@
         <v>113</v>
       </c>
       <c r="B63" s="27"/>
-      <c r="C63" s="51"/>
-      <c r="D63" s="51"/>
+      <c r="C63" s="50"/>
+      <c r="D63" s="50"/>
       <c r="E63" s="24"/>
-      <c r="F63" s="43"/>
-      <c r="G63" s="43"/>
+      <c r="F63" s="42"/>
+      <c r="G63" s="42"/>
       <c r="H63" s="25"/>
       <c r="I63" s="23"/>
       <c r="J63" s="26"/>
-      <c r="K63" s="48" t="s">
+      <c r="K63" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3871,15 +3872,15 @@
         <v>114</v>
       </c>
       <c r="B64" s="27"/>
-      <c r="C64" s="51"/>
-      <c r="D64" s="51"/>
+      <c r="C64" s="50"/>
+      <c r="D64" s="50"/>
       <c r="E64" s="24"/>
-      <c r="F64" s="43"/>
-      <c r="G64" s="43"/>
+      <c r="F64" s="42"/>
+      <c r="G64" s="42"/>
       <c r="H64" s="25"/>
       <c r="I64" s="23"/>
       <c r="J64" s="26"/>
-      <c r="K64" s="48" t="s">
+      <c r="K64" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3888,15 +3889,15 @@
         <v>115</v>
       </c>
       <c r="B65" s="27"/>
-      <c r="C65" s="51"/>
-      <c r="D65" s="51"/>
+      <c r="C65" s="50"/>
+      <c r="D65" s="50"/>
       <c r="E65" s="24"/>
-      <c r="F65" s="43"/>
-      <c r="G65" s="43"/>
+      <c r="F65" s="42"/>
+      <c r="G65" s="42"/>
       <c r="H65" s="25"/>
       <c r="I65" s="23"/>
       <c r="J65" s="26"/>
-      <c r="K65" s="48" t="s">
+      <c r="K65" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3905,15 +3906,15 @@
         <v>116</v>
       </c>
       <c r="B66" s="27"/>
-      <c r="C66" s="51"/>
-      <c r="D66" s="51"/>
+      <c r="C66" s="50"/>
+      <c r="D66" s="50"/>
       <c r="E66" s="24"/>
-      <c r="F66" s="43"/>
-      <c r="G66" s="43"/>
+      <c r="F66" s="42"/>
+      <c r="G66" s="42"/>
       <c r="H66" s="25"/>
       <c r="I66" s="23"/>
       <c r="J66" s="26"/>
-      <c r="K66" s="48" t="s">
+      <c r="K66" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3922,15 +3923,15 @@
         <v>117</v>
       </c>
       <c r="B67" s="27"/>
-      <c r="C67" s="51"/>
-      <c r="D67" s="51"/>
+      <c r="C67" s="50"/>
+      <c r="D67" s="50"/>
       <c r="E67" s="24"/>
-      <c r="F67" s="43"/>
-      <c r="G67" s="43"/>
+      <c r="F67" s="42"/>
+      <c r="G67" s="42"/>
       <c r="H67" s="25"/>
       <c r="I67" s="23"/>
       <c r="J67" s="26"/>
-      <c r="K67" s="48" t="s">
+      <c r="K67" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3939,15 +3940,15 @@
         <v>118</v>
       </c>
       <c r="B68" s="27"/>
-      <c r="C68" s="51"/>
-      <c r="D68" s="51"/>
+      <c r="C68" s="50"/>
+      <c r="D68" s="50"/>
       <c r="E68" s="24"/>
-      <c r="F68" s="43"/>
-      <c r="G68" s="43"/>
+      <c r="F68" s="42"/>
+      <c r="G68" s="42"/>
       <c r="H68" s="25"/>
       <c r="I68" s="23"/>
       <c r="J68" s="26"/>
-      <c r="K68" s="48" t="s">
+      <c r="K68" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3956,15 +3957,15 @@
         <v>119</v>
       </c>
       <c r="B69" s="27"/>
-      <c r="C69" s="51"/>
-      <c r="D69" s="51"/>
+      <c r="C69" s="50"/>
+      <c r="D69" s="50"/>
       <c r="E69" s="24"/>
-      <c r="F69" s="43"/>
-      <c r="G69" s="43"/>
+      <c r="F69" s="42"/>
+      <c r="G69" s="42"/>
       <c r="H69" s="25"/>
       <c r="I69" s="23"/>
       <c r="J69" s="26"/>
-      <c r="K69" s="48" t="s">
+      <c r="K69" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3973,70 +3974,63 @@
         <v>120</v>
       </c>
       <c r="B70" s="30"/>
-      <c r="C70" s="53"/>
-      <c r="D70" s="54"/>
+      <c r="C70" s="52"/>
+      <c r="D70" s="53"/>
       <c r="E70" s="31"/>
-      <c r="F70" s="43"/>
-      <c r="G70" s="43"/>
+      <c r="F70" s="42"/>
+      <c r="G70" s="42"/>
       <c r="H70" s="32"/>
       <c r="I70" s="33"/>
       <c r="J70" s="34"/>
-      <c r="K70" s="55" t="s">
+      <c r="K70" s="54" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="71" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="63" t="s">
+      <c r="A71" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="B71" s="63"/>
-      <c r="C71" s="63"/>
-      <c r="D71" s="35"/>
-      <c r="E71" s="36"/>
-      <c r="F71" s="36"/>
-      <c r="G71" s="36"/>
+      <c r="B71" s="69"/>
+      <c r="C71" s="69"/>
+      <c r="D71" s="90"/>
+      <c r="E71" s="35"/>
+      <c r="F71" s="35"/>
+      <c r="G71" s="35"/>
       <c r="H71" s="2"/>
       <c r="I71" s="2"/>
       <c r="J71" s="2"/>
     </row>
     <row r="72" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D72" s="37" t="s">
+      <c r="D72" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="E72" s="37"/>
-      <c r="F72" s="37"/>
-      <c r="G72" s="37"/>
+      <c r="E72" s="36"/>
+      <c r="F72" s="36"/>
+      <c r="G72" s="36"/>
     </row>
     <row r="73" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G73" s="38"/>
-      <c r="H73" s="38"/>
-      <c r="I73" s="38"/>
-      <c r="J73" s="38"/>
+      <c r="G73" s="37"/>
+      <c r="H73" s="37"/>
+      <c r="I73" s="37"/>
+      <c r="J73" s="37"/>
     </row>
     <row r="74" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="39" t="s">
+      <c r="A74" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="C74" s="64"/>
-      <c r="D74" s="64"/>
-      <c r="E74" s="40"/>
-      <c r="F74" s="40"/>
-      <c r="G74" s="65" t="s">
+      <c r="C74" s="70"/>
+      <c r="D74" s="70"/>
+      <c r="E74" s="39"/>
+      <c r="F74" s="39"/>
+      <c r="G74" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="H74" s="65"/>
-      <c r="I74" s="65"/>
-      <c r="J74" s="65"/>
+      <c r="H74" s="71"/>
+      <c r="I74" s="71"/>
+      <c r="J74" s="71"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="I5:J5"/>
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="A71:C71"/>
     <mergeCell ref="C74:D74"/>
@@ -4051,6 +4045,13 @@
     <mergeCell ref="F9:G9"/>
     <mergeCell ref="H9:H10"/>
     <mergeCell ref="I9:I10"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="I5:J5"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="84" fitToHeight="0" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -4081,147 +4082,147 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="57"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="58" t="s">
+      <c r="A2" s="56"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="88" t="s">
+      <c r="D2" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="57"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="56"/>
     </row>
     <row r="3" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="89" t="s">
+      <c r="A3" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="89"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
+      <c r="J3" s="66"/>
     </row>
     <row r="4" spans="1:11" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J4" s="62"/>
+      <c r="J4" s="61"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="90"/>
-      <c r="D5" s="90"/>
-      <c r="E5" s="90"/>
-      <c r="F5" s="90"/>
-      <c r="G5" s="90"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
       <c r="H5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="67" t="s">
+      <c r="I5" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="J5" s="67"/>
+      <c r="J5" s="68"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="66"/>
-      <c r="D6" s="66"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="66"/>
-      <c r="G6" s="66"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="62"/>
       <c r="H6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="86"/>
-      <c r="J6" s="86"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="63"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="66"/>
-      <c r="D7" s="66"/>
-      <c r="E7" s="66"/>
-      <c r="F7" s="66"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
       <c r="G7" s="6"/>
       <c r="H7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="67"/>
-      <c r="J7" s="67"/>
+      <c r="I7" s="68"/>
+      <c r="J7" s="68"/>
     </row>
     <row r="8" spans="1:11" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J8" s="45"/>
+      <c r="J8" s="44"/>
     </row>
     <row r="9" spans="1:11" s="8" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="68" t="s">
+      <c r="A9" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="70" t="s">
+      <c r="B9" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="72" t="s">
+      <c r="C9" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="74" t="s">
+      <c r="D9" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="76" t="s">
+      <c r="E9" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="84" t="s">
+      <c r="F9" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="85"/>
-      <c r="H9" s="78" t="s">
+      <c r="G9" s="89"/>
+      <c r="H9" s="82" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="80" t="s">
+      <c r="I9" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="J9" s="82" t="s">
+      <c r="J9" s="86" t="s">
         <v>17</v>
       </c>
-      <c r="K9" s="83"/>
+      <c r="K9" s="87"/>
     </row>
     <row r="10" spans="1:11" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="69"/>
-      <c r="B10" s="71"/>
-      <c r="C10" s="73"/>
-      <c r="D10" s="75"/>
-      <c r="E10" s="77"/>
-      <c r="F10" s="46" t="s">
+      <c r="A10" s="73"/>
+      <c r="B10" s="75"/>
+      <c r="C10" s="77"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="81"/>
+      <c r="F10" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="G10" s="42" t="s">
+      <c r="G10" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="H10" s="79"/>
-      <c r="I10" s="81"/>
+      <c r="H10" s="83"/>
+      <c r="I10" s="85"/>
       <c r="J10" s="9" t="s">
         <v>18</v>
       </c>
@@ -4237,12 +4238,12 @@
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
       <c r="E11" s="14"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
       <c r="H11" s="15"/>
-      <c r="I11" s="47"/>
+      <c r="I11" s="46"/>
       <c r="J11" s="16"/>
-      <c r="K11" s="48" t="s">
+      <c r="K11" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4254,12 +4255,12 @@
       <c r="C12" s="19"/>
       <c r="D12" s="19"/>
       <c r="E12" s="20"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
       <c r="H12" s="21"/>
-      <c r="I12" s="49"/>
+      <c r="I12" s="48"/>
       <c r="J12" s="22"/>
-      <c r="K12" s="48" t="s">
+      <c r="K12" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4271,12 +4272,12 @@
       <c r="C13" s="19"/>
       <c r="D13" s="19"/>
       <c r="E13" s="20"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
       <c r="H13" s="21"/>
-      <c r="I13" s="49"/>
+      <c r="I13" s="48"/>
       <c r="J13" s="22"/>
-      <c r="K13" s="48" t="s">
+      <c r="K13" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4288,12 +4289,12 @@
       <c r="C14" s="19"/>
       <c r="D14" s="19"/>
       <c r="E14" s="20"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
       <c r="H14" s="21"/>
-      <c r="I14" s="49"/>
+      <c r="I14" s="48"/>
       <c r="J14" s="22"/>
-      <c r="K14" s="48" t="s">
+      <c r="K14" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4305,12 +4306,12 @@
       <c r="C15" s="19"/>
       <c r="D15" s="19"/>
       <c r="E15" s="20"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="43"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="42"/>
       <c r="H15" s="21"/>
-      <c r="I15" s="49"/>
+      <c r="I15" s="48"/>
       <c r="J15" s="22"/>
-      <c r="K15" s="48" t="s">
+      <c r="K15" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4322,12 +4323,12 @@
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
       <c r="E16" s="20"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="43"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
       <c r="H16" s="21"/>
       <c r="I16" s="23"/>
       <c r="J16" s="22"/>
-      <c r="K16" s="48" t="s">
+      <c r="K16" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4339,12 +4340,12 @@
       <c r="C17" s="19"/>
       <c r="D17" s="19"/>
       <c r="E17" s="20"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="43"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
       <c r="H17" s="21"/>
       <c r="I17" s="23"/>
       <c r="J17" s="22"/>
-      <c r="K17" s="48" t="s">
+      <c r="K17" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4356,12 +4357,12 @@
       <c r="C18" s="19"/>
       <c r="D18" s="19"/>
       <c r="E18" s="20"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
       <c r="H18" s="21"/>
-      <c r="I18" s="49"/>
+      <c r="I18" s="48"/>
       <c r="J18" s="22"/>
-      <c r="K18" s="48" t="s">
+      <c r="K18" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4373,12 +4374,12 @@
       <c r="C19" s="19"/>
       <c r="D19" s="19"/>
       <c r="E19" s="20"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="42"/>
       <c r="H19" s="21"/>
-      <c r="I19" s="49"/>
+      <c r="I19" s="48"/>
       <c r="J19" s="22"/>
-      <c r="K19" s="48" t="s">
+      <c r="K19" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4390,12 +4391,12 @@
       <c r="C20" s="19"/>
       <c r="D20" s="19"/>
       <c r="E20" s="20"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="43"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="42"/>
       <c r="H20" s="21"/>
-      <c r="I20" s="49"/>
+      <c r="I20" s="48"/>
       <c r="J20" s="22"/>
-      <c r="K20" s="48" t="s">
+      <c r="K20" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4407,12 +4408,12 @@
       <c r="C21" s="19"/>
       <c r="D21" s="19"/>
       <c r="E21" s="20"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="43"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="42"/>
       <c r="H21" s="21"/>
-      <c r="I21" s="49"/>
+      <c r="I21" s="48"/>
       <c r="J21" s="22"/>
-      <c r="K21" s="48" t="s">
+      <c r="K21" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4424,12 +4425,12 @@
       <c r="C22" s="19"/>
       <c r="D22" s="19"/>
       <c r="E22" s="20"/>
-      <c r="F22" s="43"/>
-      <c r="G22" s="43"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="42"/>
       <c r="H22" s="21"/>
-      <c r="I22" s="49"/>
+      <c r="I22" s="48"/>
       <c r="J22" s="22"/>
-      <c r="K22" s="48" t="s">
+      <c r="K22" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4441,12 +4442,12 @@
       <c r="C23" s="19"/>
       <c r="D23" s="19"/>
       <c r="E23" s="20"/>
-      <c r="F23" s="43"/>
-      <c r="G23" s="43"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="42"/>
       <c r="H23" s="21"/>
-      <c r="I23" s="49"/>
+      <c r="I23" s="48"/>
       <c r="J23" s="22"/>
-      <c r="K23" s="48" t="s">
+      <c r="K23" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4454,16 +4455,16 @@
       <c r="A24" s="17">
         <v>134</v>
       </c>
-      <c r="B24" s="50"/>
-      <c r="C24" s="51"/>
-      <c r="D24" s="51"/>
+      <c r="B24" s="49"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="50"/>
       <c r="E24" s="20"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="43"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="42"/>
       <c r="H24" s="21"/>
-      <c r="I24" s="49"/>
-      <c r="J24" s="52"/>
-      <c r="K24" s="48" t="s">
+      <c r="I24" s="48"/>
+      <c r="J24" s="51"/>
+      <c r="K24" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4471,16 +4472,16 @@
       <c r="A25" s="11">
         <v>135</v>
       </c>
-      <c r="B25" s="50"/>
-      <c r="C25" s="51"/>
-      <c r="D25" s="51"/>
+      <c r="B25" s="49"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="50"/>
       <c r="E25" s="20"/>
-      <c r="F25" s="43"/>
-      <c r="G25" s="43"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="42"/>
       <c r="H25" s="21"/>
-      <c r="I25" s="49"/>
-      <c r="J25" s="52"/>
-      <c r="K25" s="48" t="s">
+      <c r="I25" s="48"/>
+      <c r="J25" s="51"/>
+      <c r="K25" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4488,16 +4489,16 @@
       <c r="A26" s="17">
         <v>136</v>
       </c>
-      <c r="B26" s="50"/>
-      <c r="C26" s="51"/>
-      <c r="D26" s="51"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="50"/>
       <c r="E26" s="24"/>
-      <c r="F26" s="43"/>
-      <c r="G26" s="43"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="42"/>
       <c r="H26" s="25"/>
       <c r="I26" s="23"/>
       <c r="J26" s="26"/>
-      <c r="K26" s="48" t="s">
+      <c r="K26" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4505,16 +4506,16 @@
       <c r="A27" s="11">
         <v>137</v>
       </c>
-      <c r="B27" s="50"/>
-      <c r="C27" s="51"/>
-      <c r="D27" s="51"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="50"/>
+      <c r="D27" s="50"/>
       <c r="E27" s="20"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="43"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
       <c r="H27" s="21"/>
-      <c r="I27" s="49"/>
-      <c r="J27" s="52"/>
-      <c r="K27" s="48" t="s">
+      <c r="I27" s="48"/>
+      <c r="J27" s="51"/>
+      <c r="K27" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4522,16 +4523,16 @@
       <c r="A28" s="17">
         <v>138</v>
       </c>
-      <c r="B28" s="50"/>
-      <c r="C28" s="51"/>
-      <c r="D28" s="51"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="50"/>
       <c r="E28" s="24"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
+      <c r="F28" s="42"/>
+      <c r="G28" s="42"/>
       <c r="H28" s="25"/>
       <c r="I28" s="23"/>
       <c r="J28" s="26"/>
-      <c r="K28" s="48" t="s">
+      <c r="K28" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4539,16 +4540,16 @@
       <c r="A29" s="11">
         <v>139</v>
       </c>
-      <c r="B29" s="50"/>
-      <c r="C29" s="51"/>
-      <c r="D29" s="51"/>
+      <c r="B29" s="49"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="50"/>
       <c r="E29" s="24"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="43"/>
+      <c r="F29" s="42"/>
+      <c r="G29" s="42"/>
       <c r="H29" s="25"/>
       <c r="I29" s="23"/>
       <c r="J29" s="26"/>
-      <c r="K29" s="48" t="s">
+      <c r="K29" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4556,16 +4557,16 @@
       <c r="A30" s="17">
         <v>140</v>
       </c>
-      <c r="B30" s="50"/>
-      <c r="C30" s="51"/>
-      <c r="D30" s="51"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="50"/>
+      <c r="D30" s="50"/>
       <c r="E30" s="24"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="43"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="42"/>
       <c r="H30" s="25"/>
       <c r="I30" s="23"/>
       <c r="J30" s="26"/>
-      <c r="K30" s="48" t="s">
+      <c r="K30" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4573,16 +4574,16 @@
       <c r="A31" s="11">
         <v>141</v>
       </c>
-      <c r="B31" s="50"/>
-      <c r="C31" s="51"/>
-      <c r="D31" s="51"/>
+      <c r="B31" s="49"/>
+      <c r="C31" s="50"/>
+      <c r="D31" s="50"/>
       <c r="E31" s="24"/>
-      <c r="F31" s="43"/>
-      <c r="G31" s="43"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="42"/>
       <c r="H31" s="25"/>
       <c r="I31" s="23"/>
       <c r="J31" s="26"/>
-      <c r="K31" s="48" t="s">
+      <c r="K31" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4590,16 +4591,16 @@
       <c r="A32" s="17">
         <v>142</v>
       </c>
-      <c r="B32" s="50"/>
-      <c r="C32" s="51"/>
-      <c r="D32" s="51"/>
+      <c r="B32" s="49"/>
+      <c r="C32" s="50"/>
+      <c r="D32" s="50"/>
       <c r="E32" s="20"/>
-      <c r="F32" s="43"/>
-      <c r="G32" s="43"/>
+      <c r="F32" s="42"/>
+      <c r="G32" s="42"/>
       <c r="H32" s="21"/>
-      <c r="I32" s="49"/>
-      <c r="J32" s="52"/>
-      <c r="K32" s="48" t="s">
+      <c r="I32" s="48"/>
+      <c r="J32" s="51"/>
+      <c r="K32" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4607,16 +4608,16 @@
       <c r="A33" s="11">
         <v>143</v>
       </c>
-      <c r="B33" s="50"/>
-      <c r="C33" s="51"/>
-      <c r="D33" s="51"/>
+      <c r="B33" s="49"/>
+      <c r="C33" s="50"/>
+      <c r="D33" s="50"/>
       <c r="E33" s="20"/>
-      <c r="F33" s="43"/>
-      <c r="G33" s="43"/>
+      <c r="F33" s="42"/>
+      <c r="G33" s="42"/>
       <c r="H33" s="21"/>
-      <c r="I33" s="49"/>
-      <c r="J33" s="52"/>
-      <c r="K33" s="48" t="s">
+      <c r="I33" s="48"/>
+      <c r="J33" s="51"/>
+      <c r="K33" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4624,16 +4625,16 @@
       <c r="A34" s="17">
         <v>144</v>
       </c>
-      <c r="B34" s="50"/>
-      <c r="C34" s="51"/>
-      <c r="D34" s="51"/>
+      <c r="B34" s="49"/>
+      <c r="C34" s="50"/>
+      <c r="D34" s="50"/>
       <c r="E34" s="24"/>
-      <c r="F34" s="43"/>
-      <c r="G34" s="43"/>
+      <c r="F34" s="42"/>
+      <c r="G34" s="42"/>
       <c r="H34" s="25"/>
       <c r="I34" s="23"/>
       <c r="J34" s="26"/>
-      <c r="K34" s="48" t="s">
+      <c r="K34" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4641,16 +4642,16 @@
       <c r="A35" s="11">
         <v>145</v>
       </c>
-      <c r="B35" s="50"/>
-      <c r="C35" s="51"/>
-      <c r="D35" s="51"/>
+      <c r="B35" s="49"/>
+      <c r="C35" s="50"/>
+      <c r="D35" s="50"/>
       <c r="E35" s="20"/>
-      <c r="F35" s="43"/>
-      <c r="G35" s="43"/>
+      <c r="F35" s="42"/>
+      <c r="G35" s="42"/>
       <c r="H35" s="21"/>
-      <c r="I35" s="49"/>
-      <c r="J35" s="52"/>
-      <c r="K35" s="48" t="s">
+      <c r="I35" s="48"/>
+      <c r="J35" s="51"/>
+      <c r="K35" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4658,16 +4659,16 @@
       <c r="A36" s="17">
         <v>146</v>
       </c>
-      <c r="B36" s="50"/>
-      <c r="C36" s="51"/>
-      <c r="D36" s="51"/>
+      <c r="B36" s="49"/>
+      <c r="C36" s="50"/>
+      <c r="D36" s="50"/>
       <c r="E36" s="24"/>
-      <c r="F36" s="43"/>
-      <c r="G36" s="43"/>
+      <c r="F36" s="42"/>
+      <c r="G36" s="42"/>
       <c r="H36" s="25"/>
       <c r="I36" s="23"/>
       <c r="J36" s="26"/>
-      <c r="K36" s="48" t="s">
+      <c r="K36" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4675,16 +4676,16 @@
       <c r="A37" s="11">
         <v>147</v>
       </c>
-      <c r="B37" s="50"/>
-      <c r="C37" s="51"/>
-      <c r="D37" s="51"/>
+      <c r="B37" s="49"/>
+      <c r="C37" s="50"/>
+      <c r="D37" s="50"/>
       <c r="E37" s="24"/>
-      <c r="F37" s="43"/>
-      <c r="G37" s="43"/>
+      <c r="F37" s="42"/>
+      <c r="G37" s="42"/>
       <c r="H37" s="25"/>
       <c r="I37" s="23"/>
       <c r="J37" s="26"/>
-      <c r="K37" s="48" t="s">
+      <c r="K37" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4692,16 +4693,16 @@
       <c r="A38" s="17">
         <v>148</v>
       </c>
-      <c r="B38" s="50"/>
-      <c r="C38" s="51"/>
-      <c r="D38" s="51"/>
+      <c r="B38" s="49"/>
+      <c r="C38" s="50"/>
+      <c r="D38" s="50"/>
       <c r="E38" s="24"/>
-      <c r="F38" s="43"/>
-      <c r="G38" s="43"/>
+      <c r="F38" s="42"/>
+      <c r="G38" s="42"/>
       <c r="H38" s="25"/>
       <c r="I38" s="23"/>
       <c r="J38" s="26"/>
-      <c r="K38" s="48" t="s">
+      <c r="K38" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4709,16 +4710,16 @@
       <c r="A39" s="11">
         <v>149</v>
       </c>
-      <c r="B39" s="50"/>
-      <c r="C39" s="51"/>
-      <c r="D39" s="51"/>
+      <c r="B39" s="49"/>
+      <c r="C39" s="50"/>
+      <c r="D39" s="50"/>
       <c r="E39" s="20"/>
-      <c r="F39" s="43"/>
-      <c r="G39" s="43"/>
+      <c r="F39" s="42"/>
+      <c r="G39" s="42"/>
       <c r="H39" s="21"/>
-      <c r="I39" s="49"/>
-      <c r="J39" s="52"/>
-      <c r="K39" s="48" t="s">
+      <c r="I39" s="48"/>
+      <c r="J39" s="51"/>
+      <c r="K39" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4726,16 +4727,16 @@
       <c r="A40" s="17">
         <v>150</v>
       </c>
-      <c r="B40" s="50"/>
-      <c r="C40" s="51"/>
-      <c r="D40" s="51"/>
+      <c r="B40" s="49"/>
+      <c r="C40" s="50"/>
+      <c r="D40" s="50"/>
       <c r="E40" s="20"/>
-      <c r="F40" s="43"/>
-      <c r="G40" s="43"/>
+      <c r="F40" s="42"/>
+      <c r="G40" s="42"/>
       <c r="H40" s="21"/>
-      <c r="I40" s="49"/>
-      <c r="J40" s="52"/>
-      <c r="K40" s="48" t="s">
+      <c r="I40" s="48"/>
+      <c r="J40" s="51"/>
+      <c r="K40" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4743,16 +4744,16 @@
       <c r="A41" s="11">
         <v>151</v>
       </c>
-      <c r="B41" s="50"/>
-      <c r="C41" s="51"/>
-      <c r="D41" s="51"/>
+      <c r="B41" s="49"/>
+      <c r="C41" s="50"/>
+      <c r="D41" s="50"/>
       <c r="E41" s="20"/>
-      <c r="F41" s="43"/>
-      <c r="G41" s="43"/>
+      <c r="F41" s="42"/>
+      <c r="G41" s="42"/>
       <c r="H41" s="21"/>
-      <c r="I41" s="49"/>
-      <c r="J41" s="52"/>
-      <c r="K41" s="48" t="s">
+      <c r="I41" s="48"/>
+      <c r="J41" s="51"/>
+      <c r="K41" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4760,16 +4761,16 @@
       <c r="A42" s="17">
         <v>152</v>
       </c>
-      <c r="B42" s="50"/>
-      <c r="C42" s="51"/>
-      <c r="D42" s="51"/>
+      <c r="B42" s="49"/>
+      <c r="C42" s="50"/>
+      <c r="D42" s="50"/>
       <c r="E42" s="24"/>
-      <c r="F42" s="43"/>
-      <c r="G42" s="43"/>
+      <c r="F42" s="42"/>
+      <c r="G42" s="42"/>
       <c r="H42" s="25"/>
       <c r="I42" s="23"/>
       <c r="J42" s="26"/>
-      <c r="K42" s="48" t="s">
+      <c r="K42" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4777,16 +4778,16 @@
       <c r="A43" s="11">
         <v>153</v>
       </c>
-      <c r="B43" s="50"/>
-      <c r="C43" s="51"/>
-      <c r="D43" s="51"/>
+      <c r="B43" s="49"/>
+      <c r="C43" s="50"/>
+      <c r="D43" s="50"/>
       <c r="E43" s="20"/>
-      <c r="F43" s="43"/>
-      <c r="G43" s="43"/>
+      <c r="F43" s="42"/>
+      <c r="G43" s="42"/>
       <c r="H43" s="21"/>
-      <c r="I43" s="49"/>
-      <c r="J43" s="52"/>
-      <c r="K43" s="48" t="s">
+      <c r="I43" s="48"/>
+      <c r="J43" s="51"/>
+      <c r="K43" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4794,16 +4795,16 @@
       <c r="A44" s="17">
         <v>154</v>
       </c>
-      <c r="B44" s="50"/>
-      <c r="C44" s="51"/>
-      <c r="D44" s="51"/>
+      <c r="B44" s="49"/>
+      <c r="C44" s="50"/>
+      <c r="D44" s="50"/>
       <c r="E44" s="24"/>
-      <c r="F44" s="43"/>
-      <c r="G44" s="43"/>
+      <c r="F44" s="42"/>
+      <c r="G44" s="42"/>
       <c r="H44" s="25"/>
       <c r="I44" s="23"/>
       <c r="J44" s="26"/>
-      <c r="K44" s="48" t="s">
+      <c r="K44" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4811,16 +4812,16 @@
       <c r="A45" s="11">
         <v>155</v>
       </c>
-      <c r="B45" s="50"/>
-      <c r="C45" s="51"/>
-      <c r="D45" s="51"/>
+      <c r="B45" s="49"/>
+      <c r="C45" s="50"/>
+      <c r="D45" s="50"/>
       <c r="E45" s="20"/>
-      <c r="F45" s="43"/>
-      <c r="G45" s="43"/>
+      <c r="F45" s="42"/>
+      <c r="G45" s="42"/>
       <c r="H45" s="21"/>
-      <c r="I45" s="49"/>
-      <c r="J45" s="52"/>
-      <c r="K45" s="48" t="s">
+      <c r="I45" s="48"/>
+      <c r="J45" s="51"/>
+      <c r="K45" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4829,15 +4830,15 @@
         <v>156</v>
       </c>
       <c r="B46" s="27"/>
-      <c r="C46" s="51"/>
-      <c r="D46" s="51"/>
+      <c r="C46" s="50"/>
+      <c r="D46" s="50"/>
       <c r="E46" s="24"/>
-      <c r="F46" s="43"/>
-      <c r="G46" s="43"/>
+      <c r="F46" s="42"/>
+      <c r="G46" s="42"/>
       <c r="H46" s="25"/>
       <c r="I46" s="23"/>
       <c r="J46" s="26"/>
-      <c r="K46" s="48" t="s">
+      <c r="K46" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4846,15 +4847,15 @@
         <v>157</v>
       </c>
       <c r="B47" s="27"/>
-      <c r="C47" s="51"/>
-      <c r="D47" s="51"/>
+      <c r="C47" s="50"/>
+      <c r="D47" s="50"/>
       <c r="E47" s="24"/>
-      <c r="F47" s="43"/>
-      <c r="G47" s="43"/>
+      <c r="F47" s="42"/>
+      <c r="G47" s="42"/>
       <c r="H47" s="25"/>
       <c r="I47" s="23"/>
       <c r="J47" s="26"/>
-      <c r="K47" s="48" t="s">
+      <c r="K47" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4863,15 +4864,15 @@
         <v>158</v>
       </c>
       <c r="B48" s="27"/>
-      <c r="C48" s="51"/>
-      <c r="D48" s="51"/>
+      <c r="C48" s="50"/>
+      <c r="D48" s="50"/>
       <c r="E48" s="24"/>
-      <c r="F48" s="43"/>
-      <c r="G48" s="43"/>
+      <c r="F48" s="42"/>
+      <c r="G48" s="42"/>
       <c r="H48" s="25"/>
       <c r="I48" s="23"/>
       <c r="J48" s="26"/>
-      <c r="K48" s="48" t="s">
+      <c r="K48" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4880,15 +4881,15 @@
         <v>159</v>
       </c>
       <c r="B49" s="27"/>
-      <c r="C49" s="51"/>
-      <c r="D49" s="51"/>
+      <c r="C49" s="50"/>
+      <c r="D49" s="50"/>
       <c r="E49" s="24"/>
-      <c r="F49" s="43"/>
-      <c r="G49" s="43"/>
+      <c r="F49" s="42"/>
+      <c r="G49" s="42"/>
       <c r="H49" s="25"/>
       <c r="I49" s="23"/>
       <c r="J49" s="26"/>
-      <c r="K49" s="48" t="s">
+      <c r="K49" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4897,15 +4898,15 @@
         <v>160</v>
       </c>
       <c r="B50" s="27"/>
-      <c r="C50" s="51"/>
-      <c r="D50" s="51"/>
+      <c r="C50" s="50"/>
+      <c r="D50" s="50"/>
       <c r="E50" s="24"/>
-      <c r="F50" s="43"/>
-      <c r="G50" s="43"/>
+      <c r="F50" s="42"/>
+      <c r="G50" s="42"/>
       <c r="H50" s="25"/>
       <c r="I50" s="23"/>
       <c r="J50" s="26"/>
-      <c r="K50" s="48" t="s">
+      <c r="K50" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4914,15 +4915,15 @@
         <v>161</v>
       </c>
       <c r="B51" s="27"/>
-      <c r="C51" s="51"/>
-      <c r="D51" s="51"/>
+      <c r="C51" s="50"/>
+      <c r="D51" s="50"/>
       <c r="E51" s="24"/>
-      <c r="F51" s="43"/>
-      <c r="G51" s="43"/>
+      <c r="F51" s="42"/>
+      <c r="G51" s="42"/>
       <c r="H51" s="25"/>
       <c r="I51" s="23"/>
       <c r="J51" s="26"/>
-      <c r="K51" s="48" t="s">
+      <c r="K51" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4931,15 +4932,15 @@
         <v>162</v>
       </c>
       <c r="B52" s="27"/>
-      <c r="C52" s="51"/>
-      <c r="D52" s="51"/>
+      <c r="C52" s="50"/>
+      <c r="D52" s="50"/>
       <c r="E52" s="24"/>
-      <c r="F52" s="43"/>
-      <c r="G52" s="43"/>
+      <c r="F52" s="42"/>
+      <c r="G52" s="42"/>
       <c r="H52" s="25"/>
       <c r="I52" s="23"/>
       <c r="J52" s="26"/>
-      <c r="K52" s="48" t="s">
+      <c r="K52" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4948,15 +4949,15 @@
         <v>163</v>
       </c>
       <c r="B53" s="27"/>
-      <c r="C53" s="51"/>
-      <c r="D53" s="51"/>
+      <c r="C53" s="50"/>
+      <c r="D53" s="50"/>
       <c r="E53" s="24"/>
-      <c r="F53" s="43"/>
-      <c r="G53" s="43"/>
+      <c r="F53" s="42"/>
+      <c r="G53" s="42"/>
       <c r="H53" s="25"/>
       <c r="I53" s="23"/>
       <c r="J53" s="26"/>
-      <c r="K53" s="48" t="s">
+      <c r="K53" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4965,15 +4966,15 @@
         <v>164</v>
       </c>
       <c r="B54" s="27"/>
-      <c r="C54" s="51"/>
-      <c r="D54" s="51"/>
+      <c r="C54" s="50"/>
+      <c r="D54" s="50"/>
       <c r="E54" s="24"/>
-      <c r="F54" s="43"/>
-      <c r="G54" s="43"/>
+      <c r="F54" s="42"/>
+      <c r="G54" s="42"/>
       <c r="H54" s="25"/>
       <c r="I54" s="23"/>
       <c r="J54" s="26"/>
-      <c r="K54" s="48" t="s">
+      <c r="K54" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4982,15 +4983,15 @@
         <v>165</v>
       </c>
       <c r="B55" s="27"/>
-      <c r="C55" s="51"/>
-      <c r="D55" s="51"/>
+      <c r="C55" s="50"/>
+      <c r="D55" s="50"/>
       <c r="E55" s="24"/>
-      <c r="F55" s="43"/>
-      <c r="G55" s="43"/>
+      <c r="F55" s="42"/>
+      <c r="G55" s="42"/>
       <c r="H55" s="25"/>
       <c r="I55" s="23"/>
       <c r="J55" s="26"/>
-      <c r="K55" s="48" t="s">
+      <c r="K55" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4999,15 +5000,15 @@
         <v>166</v>
       </c>
       <c r="B56" s="27"/>
-      <c r="C56" s="51"/>
-      <c r="D56" s="51"/>
+      <c r="C56" s="50"/>
+      <c r="D56" s="50"/>
       <c r="E56" s="24"/>
-      <c r="F56" s="43"/>
-      <c r="G56" s="43"/>
+      <c r="F56" s="42"/>
+      <c r="G56" s="42"/>
       <c r="H56" s="25"/>
       <c r="I56" s="23"/>
       <c r="J56" s="26"/>
-      <c r="K56" s="48" t="s">
+      <c r="K56" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -5016,15 +5017,15 @@
         <v>167</v>
       </c>
       <c r="B57" s="27"/>
-      <c r="C57" s="51"/>
-      <c r="D57" s="51"/>
+      <c r="C57" s="50"/>
+      <c r="D57" s="50"/>
       <c r="E57" s="24"/>
-      <c r="F57" s="43"/>
-      <c r="G57" s="43"/>
+      <c r="F57" s="42"/>
+      <c r="G57" s="42"/>
       <c r="H57" s="25"/>
       <c r="I57" s="23"/>
       <c r="J57" s="26"/>
-      <c r="K57" s="48" t="s">
+      <c r="K57" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -5033,15 +5034,15 @@
         <v>168</v>
       </c>
       <c r="B58" s="27"/>
-      <c r="C58" s="51"/>
-      <c r="D58" s="51"/>
+      <c r="C58" s="50"/>
+      <c r="D58" s="50"/>
       <c r="E58" s="24"/>
-      <c r="F58" s="43"/>
-      <c r="G58" s="43"/>
+      <c r="F58" s="42"/>
+      <c r="G58" s="42"/>
       <c r="H58" s="25"/>
       <c r="I58" s="23"/>
       <c r="J58" s="26"/>
-      <c r="K58" s="48" t="s">
+      <c r="K58" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -5050,15 +5051,15 @@
         <v>169</v>
       </c>
       <c r="B59" s="27"/>
-      <c r="C59" s="51"/>
-      <c r="D59" s="51"/>
+      <c r="C59" s="50"/>
+      <c r="D59" s="50"/>
       <c r="E59" s="24"/>
-      <c r="F59" s="43"/>
-      <c r="G59" s="43"/>
+      <c r="F59" s="42"/>
+      <c r="G59" s="42"/>
       <c r="H59" s="25"/>
       <c r="I59" s="23"/>
       <c r="J59" s="26"/>
-      <c r="K59" s="48" t="s">
+      <c r="K59" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -5067,15 +5068,15 @@
         <v>170</v>
       </c>
       <c r="B60" s="27"/>
-      <c r="C60" s="51"/>
-      <c r="D60" s="51"/>
+      <c r="C60" s="50"/>
+      <c r="D60" s="50"/>
       <c r="E60" s="24"/>
-      <c r="F60" s="43"/>
-      <c r="G60" s="43"/>
+      <c r="F60" s="42"/>
+      <c r="G60" s="42"/>
       <c r="H60" s="25"/>
       <c r="I60" s="23"/>
       <c r="J60" s="26"/>
-      <c r="K60" s="48" t="s">
+      <c r="K60" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -5084,15 +5085,15 @@
         <v>171</v>
       </c>
       <c r="B61" s="27"/>
-      <c r="C61" s="51"/>
-      <c r="D61" s="51"/>
+      <c r="C61" s="50"/>
+      <c r="D61" s="50"/>
       <c r="E61" s="24"/>
-      <c r="F61" s="43"/>
-      <c r="G61" s="43"/>
+      <c r="F61" s="42"/>
+      <c r="G61" s="42"/>
       <c r="H61" s="25"/>
       <c r="I61" s="23"/>
       <c r="J61" s="26"/>
-      <c r="K61" s="48" t="s">
+      <c r="K61" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -5101,15 +5102,15 @@
         <v>172</v>
       </c>
       <c r="B62" s="27"/>
-      <c r="C62" s="51"/>
-      <c r="D62" s="51"/>
+      <c r="C62" s="50"/>
+      <c r="D62" s="50"/>
       <c r="E62" s="24"/>
-      <c r="F62" s="43"/>
-      <c r="G62" s="43"/>
+      <c r="F62" s="42"/>
+      <c r="G62" s="42"/>
       <c r="H62" s="25"/>
       <c r="I62" s="23"/>
       <c r="J62" s="26"/>
-      <c r="K62" s="48" t="s">
+      <c r="K62" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -5118,15 +5119,15 @@
         <v>173</v>
       </c>
       <c r="B63" s="27"/>
-      <c r="C63" s="51"/>
-      <c r="D63" s="51"/>
+      <c r="C63" s="50"/>
+      <c r="D63" s="50"/>
       <c r="E63" s="24"/>
-      <c r="F63" s="43"/>
-      <c r="G63" s="43"/>
+      <c r="F63" s="42"/>
+      <c r="G63" s="42"/>
       <c r="H63" s="25"/>
       <c r="I63" s="23"/>
       <c r="J63" s="26"/>
-      <c r="K63" s="48" t="s">
+      <c r="K63" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -5135,15 +5136,15 @@
         <v>174</v>
       </c>
       <c r="B64" s="27"/>
-      <c r="C64" s="51"/>
-      <c r="D64" s="51"/>
+      <c r="C64" s="50"/>
+      <c r="D64" s="50"/>
       <c r="E64" s="24"/>
-      <c r="F64" s="43"/>
-      <c r="G64" s="43"/>
+      <c r="F64" s="42"/>
+      <c r="G64" s="42"/>
       <c r="H64" s="25"/>
       <c r="I64" s="23"/>
       <c r="J64" s="26"/>
-      <c r="K64" s="48" t="s">
+      <c r="K64" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -5152,15 +5153,15 @@
         <v>175</v>
       </c>
       <c r="B65" s="27"/>
-      <c r="C65" s="51"/>
-      <c r="D65" s="51"/>
+      <c r="C65" s="50"/>
+      <c r="D65" s="50"/>
       <c r="E65" s="24"/>
-      <c r="F65" s="43"/>
-      <c r="G65" s="43"/>
+      <c r="F65" s="42"/>
+      <c r="G65" s="42"/>
       <c r="H65" s="25"/>
       <c r="I65" s="23"/>
       <c r="J65" s="26"/>
-      <c r="K65" s="48" t="s">
+      <c r="K65" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -5169,15 +5170,15 @@
         <v>176</v>
       </c>
       <c r="B66" s="27"/>
-      <c r="C66" s="51"/>
-      <c r="D66" s="51"/>
+      <c r="C66" s="50"/>
+      <c r="D66" s="50"/>
       <c r="E66" s="24"/>
-      <c r="F66" s="43"/>
-      <c r="G66" s="43"/>
+      <c r="F66" s="42"/>
+      <c r="G66" s="42"/>
       <c r="H66" s="25"/>
       <c r="I66" s="23"/>
       <c r="J66" s="26"/>
-      <c r="K66" s="48" t="s">
+      <c r="K66" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -5186,15 +5187,15 @@
         <v>177</v>
       </c>
       <c r="B67" s="27"/>
-      <c r="C67" s="51"/>
-      <c r="D67" s="51"/>
+      <c r="C67" s="50"/>
+      <c r="D67" s="50"/>
       <c r="E67" s="24"/>
-      <c r="F67" s="43"/>
-      <c r="G67" s="43"/>
+      <c r="F67" s="42"/>
+      <c r="G67" s="42"/>
       <c r="H67" s="25"/>
       <c r="I67" s="23"/>
       <c r="J67" s="26"/>
-      <c r="K67" s="48" t="s">
+      <c r="K67" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -5203,15 +5204,15 @@
         <v>178</v>
       </c>
       <c r="B68" s="27"/>
-      <c r="C68" s="51"/>
-      <c r="D68" s="51"/>
+      <c r="C68" s="50"/>
+      <c r="D68" s="50"/>
       <c r="E68" s="24"/>
-      <c r="F68" s="43"/>
-      <c r="G68" s="43"/>
+      <c r="F68" s="42"/>
+      <c r="G68" s="42"/>
       <c r="H68" s="25"/>
       <c r="I68" s="23"/>
       <c r="J68" s="26"/>
-      <c r="K68" s="48" t="s">
+      <c r="K68" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -5220,15 +5221,15 @@
         <v>179</v>
       </c>
       <c r="B69" s="27"/>
-      <c r="C69" s="51"/>
-      <c r="D69" s="51"/>
+      <c r="C69" s="50"/>
+      <c r="D69" s="50"/>
       <c r="E69" s="24"/>
-      <c r="F69" s="43"/>
-      <c r="G69" s="43"/>
+      <c r="F69" s="42"/>
+      <c r="G69" s="42"/>
       <c r="H69" s="25"/>
       <c r="I69" s="23"/>
       <c r="J69" s="26"/>
-      <c r="K69" s="48" t="s">
+      <c r="K69" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -5237,63 +5238,70 @@
         <v>180</v>
       </c>
       <c r="B70" s="30"/>
-      <c r="C70" s="53"/>
-      <c r="D70" s="54"/>
+      <c r="C70" s="52"/>
+      <c r="D70" s="53"/>
       <c r="E70" s="31"/>
-      <c r="F70" s="43"/>
-      <c r="G70" s="43"/>
+      <c r="F70" s="42"/>
+      <c r="G70" s="42"/>
       <c r="H70" s="32"/>
       <c r="I70" s="33"/>
       <c r="J70" s="34"/>
-      <c r="K70" s="55" t="s">
+      <c r="K70" s="54" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="71" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="63" t="s">
+      <c r="A71" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="B71" s="63"/>
-      <c r="C71" s="63"/>
-      <c r="D71" s="35"/>
-      <c r="E71" s="36"/>
-      <c r="F71" s="36"/>
-      <c r="G71" s="36"/>
+      <c r="B71" s="69"/>
+      <c r="C71" s="69"/>
+      <c r="D71" s="90"/>
+      <c r="E71" s="35"/>
+      <c r="F71" s="35"/>
+      <c r="G71" s="35"/>
       <c r="H71" s="2"/>
       <c r="I71" s="2"/>
       <c r="J71" s="2"/>
     </row>
     <row r="72" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D72" s="37" t="s">
+      <c r="D72" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="E72" s="37"/>
-      <c r="F72" s="37"/>
-      <c r="G72" s="37"/>
+      <c r="E72" s="36"/>
+      <c r="F72" s="36"/>
+      <c r="G72" s="36"/>
     </row>
     <row r="73" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G73" s="38"/>
-      <c r="H73" s="38"/>
-      <c r="I73" s="38"/>
-      <c r="J73" s="38"/>
+      <c r="G73" s="37"/>
+      <c r="H73" s="37"/>
+      <c r="I73" s="37"/>
+      <c r="J73" s="37"/>
     </row>
     <row r="74" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="39" t="s">
+      <c r="A74" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="C74" s="64"/>
-      <c r="D74" s="64"/>
-      <c r="E74" s="45"/>
-      <c r="F74" s="45"/>
-      <c r="G74" s="65" t="s">
+      <c r="C74" s="70"/>
+      <c r="D74" s="70"/>
+      <c r="E74" s="44"/>
+      <c r="F74" s="44"/>
+      <c r="G74" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="H74" s="65"/>
-      <c r="I74" s="65"/>
-      <c r="J74" s="65"/>
+      <c r="H74" s="71"/>
+      <c r="I74" s="71"/>
+      <c r="J74" s="71"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="I5:J5"/>
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="A71:C71"/>
     <mergeCell ref="C74:D74"/>
@@ -5308,13 +5316,6 @@
     <mergeCell ref="F9:G9"/>
     <mergeCell ref="H9:H10"/>
     <mergeCell ref="I9:I10"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="I5:J5"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="84" fitToHeight="0" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>